<commit_message>
refs in cyber observables are strings, not integers remove observed_data that are patterns from the report's object_refs remove_pattern_objects as last finalize task line up CHECK_CODES update golden idioms added new message 423
</commit_message>
<xml_diff>
--- a/elevator_log_messages.xlsx
+++ b/elevator_log_messages.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmanuelle\PycharmProjects\cti-stix-elevator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpiazza/git/stix-elevator/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16335" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Error Codes - STIX Elevator" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="193">
   <si>
     <t>warn</t>
   </si>
@@ -600,13 +600,19 @@
   </si>
   <si>
     <t>set_option_value</t>
+  </si>
+  <si>
+    <t>[id] is used as a pattern, therefore it is not included as an onbserved_data instance</t>
+  </si>
+  <si>
+    <t>remove_pattern_objects</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -648,6 +654,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -723,21 +735,21 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -767,8 +779,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -882,8 +896,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -898,6 +913,7 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -912,6 +928,7 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1195,23 +1212,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="77.125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="77.1640625" style="23" customWidth="1"/>
     <col min="2" max="2" width="49" style="23" customWidth="1"/>
-    <col min="3" max="3" width="7.75" style="4" customWidth="1"/>
-    <col min="4" max="4" width="7.75" customWidth="1"/>
-    <col min="5" max="5" width="40.125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" style="23" customWidth="1"/>
     <col min="6" max="6" width="65.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
@@ -1231,7 +1248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="9"/>
@@ -1239,7 +1256,7 @@
       <c r="E2" s="20"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>81</v>
       </c>
@@ -1259,7 +1276,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>176</v>
       </c>
@@ -1277,7 +1294,7 @@
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>178</v>
       </c>
@@ -1295,7 +1312,7 @@
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>180</v>
       </c>
@@ -1313,7 +1330,7 @@
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>187</v>
       </c>
@@ -1331,7 +1348,7 @@
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>188</v>
       </c>
@@ -1349,7 +1366,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>189</v>
       </c>
@@ -1367,7 +1384,7 @@
       </c>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>84</v>
       </c>
@@ -1387,7 +1404,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>85</v>
       </c>
@@ -1405,7 +1422,7 @@
       </c>
       <c r="F11" s="14"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
         <v>87</v>
       </c>
@@ -1423,7 +1440,7 @@
       </c>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>86</v>
       </c>
@@ -1441,7 +1458,7 @@
       </c>
       <c r="F13" s="14"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>88</v>
       </c>
@@ -1459,7 +1476,7 @@
       </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>89</v>
       </c>
@@ -1477,7 +1494,7 @@
       </c>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
         <v>90</v>
       </c>
@@ -1495,7 +1512,7 @@
       </c>
       <c r="F16" s="17"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
         <v>91</v>
       </c>
@@ -1513,7 +1530,7 @@
       </c>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
         <v>92</v>
       </c>
@@ -1533,7 +1550,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>93</v>
       </c>
@@ -1553,7 +1570,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>94</v>
       </c>
@@ -1571,7 +1588,7 @@
       </c>
       <c r="F20" s="17"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>95</v>
       </c>
@@ -1589,7 +1606,7 @@
       </c>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>96</v>
       </c>
@@ -1607,7 +1624,7 @@
       </c>
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>97</v>
       </c>
@@ -1625,7 +1642,7 @@
       </c>
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>98</v>
       </c>
@@ -1643,7 +1660,7 @@
       </c>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>99</v>
       </c>
@@ -1661,7 +1678,7 @@
       </c>
       <c r="F25" s="17"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>100</v>
       </c>
@@ -1679,7 +1696,7 @@
       </c>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
         <v>101</v>
       </c>
@@ -1697,7 +1714,7 @@
       </c>
       <c r="F27" s="17"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
         <v>102</v>
       </c>
@@ -1715,7 +1732,7 @@
       </c>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
         <v>104</v>
       </c>
@@ -1733,7 +1750,7 @@
       </c>
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>103</v>
       </c>
@@ -1751,7 +1768,7 @@
       </c>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>105</v>
       </c>
@@ -1769,7 +1786,7 @@
       </c>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>106</v>
       </c>
@@ -1787,7 +1804,7 @@
       </c>
       <c r="F32" s="17"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
         <v>57</v>
       </c>
@@ -1805,7 +1822,7 @@
       </c>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>58</v>
       </c>
@@ -1823,7 +1840,7 @@
       </c>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>159</v>
       </c>
@@ -1841,7 +1858,7 @@
       </c>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
         <v>162</v>
       </c>
@@ -1859,7 +1876,7 @@
       </c>
       <c r="F36" s="17"/>
     </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
         <v>166</v>
       </c>
@@ -1877,49 +1894,49 @@
       </c>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" s="31" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="18">
+        <v>423</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="49" t="s">
+        <v>192</v>
+      </c>
+      <c r="F38" s="17"/>
+    </row>
+    <row r="39" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="31"/>
+      <c r="B39" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="29">
+      <c r="C39" s="29">
         <v>501</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D39" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E39" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F38" s="28"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="F39" s="28"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="35" t="s">
         <v>108</v>
-      </c>
-      <c r="B39" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="33">
-        <v>502</v>
-      </c>
-      <c r="D39" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="F39" s="32"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
-        <v>110</v>
       </c>
       <c r="B40" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C40" s="33">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D40" s="34" t="s">
         <v>0</v>
@@ -1929,123 +1946,123 @@
       </c>
       <c r="F40" s="32"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B41" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C41" s="33">
+        <v>503</v>
+      </c>
+      <c r="D41" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="32"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="33">
         <v>504</v>
       </c>
-      <c r="D41" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" s="35" t="s">
+      <c r="D42" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F41" s="32"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31" t="s">
+      <c r="F42" s="32"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="31"/>
+      <c r="B43" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="29">
+      <c r="C43" s="29">
         <v>505</v>
       </c>
-      <c r="D42" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" s="31" t="s">
+      <c r="D43" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="F42" s="28"/>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
+      <c r="F43" s="28"/>
+    </row>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A44" s="35" t="s">
         <v>113</v>
-      </c>
-      <c r="B43" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C43" s="33">
-        <v>506</v>
-      </c>
-      <c r="D43" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="F43" s="32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
-        <v>114</v>
       </c>
       <c r="B44" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C44" s="33">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D44" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E44" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F44" s="32"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B45" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C45" s="33">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D45" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E45" s="35" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F45" s="32"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B46" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C46" s="33">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D46" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E46" s="35" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="F46" s="32"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B47" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C47" s="33">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D47" s="34" t="s">
         <v>0</v>
@@ -2055,51 +2072,51 @@
       </c>
       <c r="F47" s="32"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="s">
-        <v>42</v>
+        <v>117</v>
       </c>
       <c r="B48" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C48" s="33">
+        <v>510</v>
+      </c>
+      <c r="D48" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" s="32"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="33">
         <v>511</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="D49" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="35" t="s">
+      <c r="E49" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F48" s="32"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="39" t="s">
+      <c r="F49" s="32"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="39" t="s">
         <v>118</v>
-      </c>
-      <c r="B49" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C49" s="37">
-        <v>601</v>
-      </c>
-      <c r="D49" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="36"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="39" t="s">
-        <v>119</v>
       </c>
       <c r="B50" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C50" s="37">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D50" s="38" t="s">
         <v>0</v>
@@ -2109,217 +2126,217 @@
       </c>
       <c r="F50" s="36"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B51" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C51" s="37">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D51" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E51" s="39" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F51" s="36"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="39" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B52" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C52" s="37">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D52" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52" s="39" t="s">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="F52" s="36"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B53" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C53" s="37">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" s="39" t="s">
         <v>122</v>
       </c>
       <c r="F53" s="36"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="39" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="B54" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C54" s="37">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="F54" s="36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="F54" s="36"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="39" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B55" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C55" s="37">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D55" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E55" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F55" s="36"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F55" s="36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="39" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="B56" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C56" s="37">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D56" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E56" s="39" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F56" s="36"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="39" t="s">
-        <v>126</v>
+        <v>45</v>
       </c>
       <c r="B57" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C57" s="37">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D57" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E57" s="39" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F57" s="36"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B58" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C58" s="37">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58" s="39" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F58" s="36"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B59" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C59" s="37">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59" s="39" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F59" s="36"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B60" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C60" s="37">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D60" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E60" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="F60" s="36" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="F60" s="36"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="39" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="B61" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C61" s="37">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D61" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="F61" s="36"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="F61" s="36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B62" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C62" s="37">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D62" s="38" t="s">
         <v>0</v>
@@ -2329,33 +2346,33 @@
       </c>
       <c r="F62" s="36"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B63" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C63" s="37">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D63" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E63" s="39" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F63" s="36"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B64" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C64" s="37">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D64" s="38" t="s">
         <v>0</v>
@@ -2365,127 +2382,125 @@
       </c>
       <c r="F64" s="36"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="39" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="B65" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C65" s="37">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D65" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="F65" s="36"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="39" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="B66" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C66" s="37">
+        <v>617</v>
+      </c>
+      <c r="D66" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="F66" s="36"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="B67" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C67" s="37">
         <v>618</v>
       </c>
-      <c r="D66" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="39" t="s">
+      <c r="D67" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="F66" s="36"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="27" t="s">
+      <c r="F67" s="36"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="27" t="s">
         <v>130</v>
-      </c>
-      <c r="B67" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C67" s="25">
-        <v>701</v>
-      </c>
-      <c r="D67" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E67" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="F67" s="24"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="27" t="s">
-        <v>121</v>
       </c>
       <c r="B68" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C68" s="25">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D68" s="26" t="s">
         <v>66</v>
       </c>
       <c r="E68" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F68" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="F68" s="24"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="27" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B69" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C69" s="25">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D69" s="26" t="s">
         <v>66</v>
       </c>
       <c r="E69" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F69" s="24"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B70" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C70" s="25">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E70" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F70" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="F70" s="24"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B71" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C71" s="25">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D71" s="26" t="s">
         <v>0</v>
@@ -2497,15 +2512,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B72" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C72" s="25">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D72" s="26" t="s">
         <v>0</v>
@@ -2514,18 +2529,18 @@
         <v>12</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B73" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C73" s="25">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D73" s="26" t="s">
         <v>0</v>
@@ -2537,15 +2552,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B74" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C74" s="25">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D74" s="26" t="s">
         <v>0</v>
@@ -2554,18 +2569,18 @@
         <v>12</v>
       </c>
       <c r="F74" s="24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B75" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C75" s="25">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D75" s="26" t="s">
         <v>0</v>
@@ -2577,501 +2592,521 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B76" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C76" s="25">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D76" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E76" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F76" s="24"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B77" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C77" s="25">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D77" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F77" s="24"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="27" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="B78" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C78" s="25">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D78" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E78" s="27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F78" s="24"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="27" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="B79" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C79" s="25">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D79" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F79" s="24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="F79" s="24"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B80" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C80" s="25">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D80" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="F80" s="24"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B81" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C81" s="25">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D81" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E81" s="27" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="F81" s="24"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B82" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C82" s="25">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D82" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E82" s="27" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F82" s="24"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="27" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B83" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C83" s="25">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D83" s="26" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F83" s="24"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="27" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="B84" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C84" s="25">
+        <v>717</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E84" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F84" s="24"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="B85" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85" s="25">
         <v>718</v>
       </c>
-      <c r="D84" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="27" t="s">
+      <c r="D85" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="F84" s="24"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="43" t="s">
+      <c r="F85" s="24"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="43" t="s">
         <v>9</v>
-      </c>
-      <c r="B85" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C85" s="41">
-        <v>801</v>
-      </c>
-      <c r="D85" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E85" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="F85" s="40"/>
-    </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A86" s="43" t="s">
-        <v>44</v>
       </c>
       <c r="B86" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C86" s="41">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D86" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E86" s="43" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="F86" s="40"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A87" s="43" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B87" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C87" s="41">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D87" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E87" s="43" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F87" s="40"/>
     </row>
-    <row r="88" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B88" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C88" s="41">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D88" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E88" s="43" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="F88" s="40"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A89" s="43" t="s">
-        <v>144</v>
+        <v>49</v>
       </c>
       <c r="B89" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C89" s="41">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D89" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E89" s="43" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F89" s="40"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="43" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
       <c r="B90" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C90" s="41">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D90" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E90" s="43" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F90" s="40"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B91" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C91" s="41">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D91" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E91" s="43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F91" s="40"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="43" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="B92" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C92" s="41">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D92" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E92" s="43" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F92" s="40"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="43" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="B93" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C93" s="41">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D93" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E93" s="43" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F93" s="40"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="43" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B94" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C94" s="41">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D94" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E94" s="43" t="s">
-        <v>165</v>
+        <v>50</v>
       </c>
       <c r="F94" s="40"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="43" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B95" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C95" s="41">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D95" s="42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" s="43" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F95" s="40"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B96" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C96" s="41">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D96" s="42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E96" s="43" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F96" s="40"/>
     </row>
-    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="43" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B97" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C97" s="41">
+        <v>812</v>
+      </c>
+      <c r="D97" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="F97" s="40"/>
+    </row>
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A98" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="B98" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C98" s="41">
         <v>813</v>
       </c>
-      <c r="D97" s="42" t="s">
+      <c r="D98" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="E97" s="43" t="s">
+      <c r="E98" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="F97" s="40"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="47" t="s">
+      <c r="F98" s="40"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="47" t="s">
         <v>30</v>
-      </c>
-      <c r="B98" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C98" s="45">
-        <v>901</v>
-      </c>
-      <c r="D98" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E98" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="F98" s="44"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="47" t="s">
-        <v>150</v>
       </c>
       <c r="B99" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C99" s="45">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D99" s="46" t="s">
         <v>66</v>
       </c>
       <c r="E99" s="47" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F99" s="44"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="47" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B100" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C100" s="45">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D100" s="46" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E100" s="47" t="s">
-        <v>29</v>
+        <v>151</v>
       </c>
       <c r="F100" s="44"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B101" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C101" s="45">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D101" s="46" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="E101" s="47" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F101" s="44"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="47" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B102" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C102" s="45">
+        <v>904</v>
+      </c>
+      <c r="D102" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E102" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F102" s="44"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="B103" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C103" s="45">
         <v>905</v>
       </c>
-      <c r="D102" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E102" s="47" t="s">
+      <c r="D103" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="F102" s="44"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="2"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="1"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="1"/>
+      <c r="F103" s="44"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="2"/>
+      <c r="B104" s="2"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="2"/>
+      <c r="F104" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:E69">

</xml_diff>

<commit_message>
Update package structure, renamed package, update unittest to work in py.test
</commit_message>
<xml_diff>
--- a/elevator_log_messages.xlsx
+++ b/elevator_log_messages.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="203">
   <si>
     <t>warn</t>
   </si>
@@ -627,6 +627,15 @@
   </si>
   <si>
     <t xml:space="preserve">convert_vulnerability, convert_indicator, </t>
+  </si>
+  <si>
+    <t>Both console and output log have disabled messages.</t>
+  </si>
+  <si>
+    <t>ElevatorOptions.__init__()</t>
+  </si>
+  <si>
+    <t>OSError [message]</t>
   </si>
 </sst>
 </file>
@@ -1234,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F108"/>
+  <dimension ref="A1:F110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1426,327 +1435,327 @@
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="11">
+        <v>209</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="11">
+        <v>210</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>84</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="15">
-        <v>301</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="15">
-        <v>302</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="14"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>87</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>71</v>
       </c>
       <c r="C13" s="15">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>71</v>
       </c>
       <c r="C14" s="15">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>71</v>
       </c>
       <c r="C15" s="15">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="15">
+        <v>304</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="14"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="15">
+        <v>305</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="15">
         <v>306</v>
       </c>
-      <c r="D16" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="13" t="s">
+      <c r="D18" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C17" s="18">
-        <v>401</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="18">
-        <v>402</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="17"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C19" s="18">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D19" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>16</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C20" s="18">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>18</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C21" s="18">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F21" s="17"/>
+        <v>17</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B22" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="18">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="17"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B23" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="18">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F23" s="17"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C24" s="18">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B25" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C25" s="18">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C26" s="18">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F26" s="17"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B27" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C27" s="18">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C28" s="18">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>0</v>
@@ -1758,49 +1767,49 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B29" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C29" s="18">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F29" s="17"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C30" s="18">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F30" s="17"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C31" s="18">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>0</v>
@@ -1812,243 +1821,245 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C32" s="18">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F32" s="17"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C33" s="18">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C34" s="18">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="F34" s="17"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C35" s="18">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>159</v>
+        <v>57</v>
       </c>
       <c r="B36" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C36" s="18">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="F36" s="17"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>162</v>
+        <v>58</v>
       </c>
       <c r="B37" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C37" s="18">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>163</v>
+        <v>56</v>
       </c>
       <c r="F37" s="17"/>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B38" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C38" s="18">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="F38" s="17"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="s">
-        <v>190</v>
+      <c r="A39" s="22" t="s">
+        <v>162</v>
       </c>
       <c r="B39" s="22" t="s">
         <v>70</v>
       </c>
       <c r="C39" s="18">
+        <v>421</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F39" s="17"/>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="18">
+        <v>422</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F40" s="17"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="49" t="s">
+        <v>190</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="18">
         <v>423</v>
       </c>
-      <c r="D39" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E39" s="50" t="s">
+      <c r="D41" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="F39" s="17"/>
-    </row>
-    <row r="40" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31" t="s">
+      <c r="F41" s="17"/>
+    </row>
+    <row r="42" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
+      <c r="B42" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C40" s="29">
+      <c r="C42" s="29">
         <v>501</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D42" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E42" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F40" s="28"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="B41" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" s="33">
-        <v>502</v>
-      </c>
-      <c r="D41" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" s="32"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="B42" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="33">
-        <v>503</v>
-      </c>
-      <c r="D42" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="32"/>
+      <c r="F42" s="28"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="35" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B43" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C43" s="33">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D43" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E43" s="35" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F43" s="32"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31" t="s">
+      <c r="A44" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="29">
-        <v>505</v>
-      </c>
-      <c r="D44" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="F44" s="28"/>
-    </row>
-    <row r="45" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C44" s="33">
+        <v>503</v>
+      </c>
+      <c r="D44" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="32"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B45" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C45" s="33">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D45" s="34" t="s">
         <v>0</v>
@@ -2056,533 +2067,527 @@
       <c r="E45" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F45" s="32" t="s">
-        <v>28</v>
-      </c>
+      <c r="F45" s="32"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="B46" s="35" t="s">
+      <c r="A46" s="31"/>
+      <c r="B46" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C46" s="33">
-        <v>507</v>
-      </c>
-      <c r="D46" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F46" s="32"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="29">
+        <v>505</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="28"/>
+    </row>
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B47" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C47" s="33">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D47" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E47" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F47" s="32"/>
+        <v>27</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B48" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C48" s="33">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D48" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E48" s="35" t="s">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="F48" s="32"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B49" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C49" s="33">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D49" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E49" s="35" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="F49" s="32"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="B50" s="35" t="s">
         <v>72</v>
       </c>
       <c r="C50" s="33">
+        <v>509</v>
+      </c>
+      <c r="D50" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F50" s="32"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="33">
+        <v>510</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F51" s="32"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="33">
         <v>511</v>
       </c>
-      <c r="D50" s="34" t="s">
+      <c r="D52" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="E50" s="35" t="s">
+      <c r="E52" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F50" s="32"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="B51" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="37">
-        <v>601</v>
-      </c>
-      <c r="D51" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E51" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="F51" s="36"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="B52" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52" s="37">
-        <v>602</v>
-      </c>
-      <c r="D52" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E52" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="F52" s="36"/>
+      <c r="F52" s="32"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B53" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C53" s="37">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D53" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E53" s="39" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F53" s="36"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="39" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B54" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C54" s="37">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" s="39" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
       <c r="F54" s="36"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="39" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B55" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C55" s="37">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D55" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E55" s="39" t="s">
-        <v>122</v>
+        <v>40</v>
       </c>
       <c r="F55" s="36"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="39" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B56" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C56" s="37">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D56" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E56" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="F56" s="36" t="s">
-        <v>24</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="F56" s="36"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B57" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C57" s="37">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D57" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" s="39" t="s">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="F57" s="36"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="39" t="s">
-        <v>45</v>
+        <v>109</v>
       </c>
       <c r="B58" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C58" s="37">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D58" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E58" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="F58" s="36"/>
+        <v>23</v>
+      </c>
+      <c r="F58" s="36" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B59" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C59" s="37">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D59" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E59" s="39" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F59" s="36"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="39" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="B60" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C60" s="37">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D60" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" s="39" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F60" s="36"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="39" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B61" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C61" s="37">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D61" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F61" s="36"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="39" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B62" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C62" s="37">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="F62" s="36" t="s">
-        <v>26</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F62" s="36"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="39" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="B63" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C63" s="37">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D63" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63" s="39" t="s">
-        <v>152</v>
+        <v>62</v>
       </c>
       <c r="F63" s="36"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="39" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="B64" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C64" s="37">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="F64" s="36"/>
+        <v>25</v>
+      </c>
+      <c r="F64" s="36" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="39" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B65" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C65" s="37">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D65" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F65" s="36"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="39" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B66" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C66" s="37">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D66" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E66" s="39" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F66" s="36"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="39" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B67" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C67" s="37">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D67" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E67" s="39" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="F67" s="36"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="39" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="B68" s="39" t="s">
         <v>75</v>
       </c>
       <c r="C68" s="37">
+        <v>616</v>
+      </c>
+      <c r="D68" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="F68" s="36"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="39" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69" s="37">
+        <v>617</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="39" t="s">
+        <v>172</v>
+      </c>
+      <c r="F69" s="36"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="B70" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70" s="37">
         <v>618</v>
       </c>
-      <c r="D68" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" s="39" t="s">
+      <c r="D70" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="F68" s="36"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B69" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C69" s="25">
-        <v>701</v>
-      </c>
-      <c r="D69" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E69" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="F69" s="24"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="B70" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C70" s="25">
-        <v>702</v>
-      </c>
-      <c r="D70" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E70" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F70" s="24" t="s">
-        <v>41</v>
-      </c>
+      <c r="F70" s="36"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B71" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C71" s="25">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D71" s="26" t="s">
         <v>66</v>
       </c>
       <c r="E71" s="27" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="F71" s="24"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="27" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B72" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C72" s="25">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E72" s="27" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B73" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C73" s="25">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E73" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F73" s="24" t="s">
-        <v>13</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F73" s="24"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B74" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C74" s="25">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="D74" s="26" t="s">
         <v>0</v>
@@ -2591,18 +2596,18 @@
         <v>12</v>
       </c>
       <c r="F74" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B75" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C75" s="25">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D75" s="26" t="s">
         <v>0</v>
@@ -2611,18 +2616,18 @@
         <v>12</v>
       </c>
       <c r="F75" s="24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B76" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C76" s="25">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D76" s="26" t="s">
         <v>0</v>
@@ -2631,18 +2636,18 @@
         <v>12</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B77" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C77" s="25">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D77" s="26" t="s">
         <v>0</v>
@@ -2651,558 +2656,598 @@
         <v>12</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B78" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C78" s="25">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D78" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E78" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F78" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B79" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C79" s="25">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D79" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="F79" s="24"/>
+        <v>12</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="27" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="B80" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C80" s="25">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D80" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F80" s="24"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B81" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C81" s="25">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D81" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E81" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F81" s="24" t="s">
-        <v>37</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F81" s="24"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="B82" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C82" s="25">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D82" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E82" s="27" t="s">
-        <v>173</v>
+        <v>27</v>
       </c>
       <c r="F82" s="24"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B83" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C83" s="25">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D83" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="F83" s="24"/>
+        <v>36</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="27" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B84" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C84" s="25">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D84" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E84" s="27" t="s">
-        <v>25</v>
+        <v>173</v>
       </c>
       <c r="F84" s="24"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="27" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="B85" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C85" s="25">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="F85" s="24"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="27" t="s">
-        <v>185</v>
+        <v>143</v>
       </c>
       <c r="B86" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C86" s="25">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="D86" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E86" s="27" t="s">
-        <v>184</v>
+        <v>25</v>
       </c>
       <c r="F86" s="24"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="27" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="B87" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C87" s="25">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D87" s="26" t="s">
         <v>66</v>
       </c>
       <c r="E87" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F87" s="24"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C88" s="25">
+        <v>718</v>
+      </c>
+      <c r="D88" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="F88" s="24"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="B89" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C89" s="25">
+        <v>719</v>
+      </c>
+      <c r="D89" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="E89" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="F87" s="24"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="B88" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C88" s="41">
-        <v>801</v>
-      </c>
-      <c r="D88" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E88" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="F88" s="40"/>
-    </row>
-    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B89" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C89" s="41">
-        <v>802</v>
-      </c>
-      <c r="D89" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E89" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="F89" s="40"/>
+      <c r="F89" s="24"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="43" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="B90" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C90" s="41">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D90" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E90" s="43" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="F90" s="40"/>
     </row>
     <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="43" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B91" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C91" s="41">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D91" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E91" s="43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F91" s="40"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="43" t="s">
-        <v>144</v>
+        <v>47</v>
       </c>
       <c r="B92" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C92" s="41">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D92" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E92" s="43" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F92" s="40"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="43" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B93" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C93" s="41">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D93" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E93" s="43" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F93" s="40"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="43" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="B94" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C94" s="41">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D94" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E94" s="43" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F94" s="40"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="43" t="s">
-        <v>145</v>
+        <v>53</v>
       </c>
       <c r="B95" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C95" s="41">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D95" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E95" s="43" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F95" s="40"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="43" t="s">
-        <v>161</v>
+        <v>55</v>
       </c>
       <c r="B96" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C96" s="41">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D96" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E96" s="43" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F96" s="40"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="43" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="B97" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C97" s="41">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D97" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E97" s="43" t="s">
-        <v>165</v>
+        <v>61</v>
       </c>
       <c r="F97" s="40"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="43" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B98" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C98" s="41">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D98" s="42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98" s="43" t="s">
-        <v>168</v>
+        <v>50</v>
       </c>
       <c r="F98" s="40"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="43" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B99" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C99" s="41">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D99" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E99" s="43" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F99" s="40"/>
     </row>
-    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="43" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B100" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C100" s="41">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="D100" s="42" t="s">
         <v>1</v>
       </c>
       <c r="E100" s="43" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="F100" s="40"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="43" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="B101" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C101" s="41">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D101" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E101" s="43" t="s">
-        <v>20</v>
+        <v>170</v>
       </c>
       <c r="F101" s="40"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="43" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="B102" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C102" s="41">
+        <v>813</v>
+      </c>
+      <c r="D102" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E102" s="43" t="s">
+        <v>175</v>
+      </c>
+      <c r="F102" s="40"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="B103" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C103" s="41">
+        <v>814</v>
+      </c>
+      <c r="D103" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F103" s="40"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="B104" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C104" s="41">
         <v>815</v>
       </c>
-      <c r="D102" s="42" t="s">
+      <c r="D104" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E102" s="43" t="s">
+      <c r="E104" s="43" t="s">
         <v>199</v>
       </c>
-      <c r="F102" s="40"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="B103" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C103" s="45">
-        <v>901</v>
-      </c>
-      <c r="D103" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E103" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="F103" s="44"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="B104" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C104" s="45">
-        <v>902</v>
-      </c>
-      <c r="D104" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E104" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="F104" s="44"/>
+      <c r="F104" s="40"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="47" t="s">
-        <v>148</v>
+        <v>30</v>
       </c>
       <c r="B105" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C105" s="45">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D105" s="46" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E105" s="47" t="s">
-        <v>29</v>
+        <v>147</v>
       </c>
       <c r="F105" s="44"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="47" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B106" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C106" s="45">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="D106" s="46" t="s">
         <v>66</v>
       </c>
       <c r="E106" s="47" t="s">
-        <v>34</v>
+        <v>151</v>
       </c>
       <c r="F106" s="44"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="47" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B107" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C107" s="45">
+        <v>903</v>
+      </c>
+      <c r="D107" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E107" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="F107" s="44"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="B108" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C108" s="45">
+        <v>904</v>
+      </c>
+      <c r="D108" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E108" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F108" s="44"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="B109" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C109" s="45">
         <v>905</v>
       </c>
-      <c r="D107" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E107" s="47" t="s">
+      <c r="D109" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E109" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="F107" s="44"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="2"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="2"/>
-      <c r="F108" s="1"/>
+      <c r="F109" s="44"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="2"/>
+      <c r="F110" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:E69">

</xml_diff>

<commit_message>
Handle Investigate default valid_from/valid_until properties on indicator (#33)
</commit_message>
<xml_diff>
--- a/elevator_log_messages.xlsx
+++ b/elevator_log_messages.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmanuelle\PycharmProjects\cti-stix-elevator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpiazza/git/cti-stix-elevator/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="19200" windowHeight="11490" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="11500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Error Codes - STIX Elevator" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="204">
   <si>
     <t>warn</t>
   </si>
@@ -636,13 +636,23 @@
   </si>
   <si>
     <t>OSError [message]</t>
+  </si>
+  <si>
+    <t>No start time for the first valid time interval is available in %s, other time intervals might be more appropriate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -693,7 +703,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -754,8 +764,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -778,158 +794,179 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="31" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="31"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="34">
+    <cellStyle name="20% - Accent2" xfId="31" builtinId="34"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -945,6 +982,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -960,6 +998,7 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1243,23 +1282,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="77.125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="77.1640625" style="23" customWidth="1"/>
     <col min="2" max="2" width="49" style="23" customWidth="1"/>
-    <col min="3" max="3" width="7.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="7.625" customWidth="1"/>
-    <col min="5" max="5" width="40.125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" style="23" customWidth="1"/>
     <col min="6" max="6" width="65.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
@@ -1279,7 +1318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="9"/>
@@ -1287,7 +1326,7 @@
       <c r="E2" s="20"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>81</v>
       </c>
@@ -1307,7 +1346,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>176</v>
       </c>
@@ -1325,7 +1364,7 @@
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>197</v>
       </c>
@@ -1343,7 +1382,7 @@
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>179</v>
       </c>
@@ -1361,7 +1400,7 @@
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>186</v>
       </c>
@@ -1379,7 +1418,7 @@
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>187</v>
       </c>
@@ -1397,7 +1436,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>188</v>
       </c>
@@ -1415,7 +1454,7 @@
       </c>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>195</v>
       </c>
@@ -1435,7 +1474,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>200</v>
       </c>
@@ -1453,7 +1492,7 @@
       </c>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>202</v>
       </c>
@@ -1471,7 +1510,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>84</v>
       </c>
@@ -1491,7 +1530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>85</v>
       </c>
@@ -1509,7 +1548,7 @@
       </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>87</v>
       </c>
@@ -1527,7 +1566,7 @@
       </c>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>86</v>
       </c>
@@ -1545,7 +1584,7 @@
       </c>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
         <v>88</v>
       </c>
@@ -1563,7 +1602,7 @@
       </c>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>89</v>
       </c>
@@ -1581,7 +1620,7 @@
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>90</v>
       </c>
@@ -1599,7 +1638,7 @@
       </c>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>91</v>
       </c>
@@ -1617,7 +1656,7 @@
       </c>
       <c r="F20" s="17"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
         <v>92</v>
       </c>
@@ -1637,7 +1676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>93</v>
       </c>
@@ -1657,7 +1696,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>94</v>
       </c>
@@ -1675,7 +1714,7 @@
       </c>
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
         <v>95</v>
       </c>
@@ -1693,7 +1732,7 @@
       </c>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>96</v>
       </c>
@@ -1711,7 +1750,7 @@
       </c>
       <c r="F25" s="17"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
         <v>97</v>
       </c>
@@ -1729,7 +1768,7 @@
       </c>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
         <v>98</v>
       </c>
@@ -1747,7 +1786,7 @@
       </c>
       <c r="F27" s="17"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
         <v>99</v>
       </c>
@@ -1765,7 +1804,7 @@
       </c>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
         <v>100</v>
       </c>
@@ -1783,7 +1822,7 @@
       </c>
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
         <v>101</v>
       </c>
@@ -1801,7 +1840,7 @@
       </c>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
         <v>102</v>
       </c>
@@ -1819,7 +1858,7 @@
       </c>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
         <v>104</v>
       </c>
@@ -1837,7 +1876,7 @@
       </c>
       <c r="F32" s="17"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
         <v>103</v>
       </c>
@@ -1855,7 +1894,7 @@
       </c>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
         <v>105</v>
       </c>
@@ -1873,7 +1912,7 @@
       </c>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
         <v>106</v>
       </c>
@@ -1891,7 +1930,7 @@
       </c>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
         <v>57</v>
       </c>
@@ -1909,7 +1948,7 @@
       </c>
       <c r="F36" s="17"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
         <v>58</v>
       </c>
@@ -1927,7 +1966,7 @@
       </c>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
         <v>159</v>
       </c>
@@ -1945,7 +1984,7 @@
       </c>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
         <v>162</v>
       </c>
@@ -1963,7 +2002,7 @@
       </c>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
         <v>166</v>
       </c>
@@ -1981,7 +2020,7 @@
       </c>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="49" t="s">
         <v>190</v>
       </c>
@@ -1999,7 +2038,7 @@
       </c>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="31"/>
       <c r="B42" s="31" t="s">
         <v>72</v>
@@ -2015,7 +2054,7 @@
       </c>
       <c r="F42" s="28"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="35" t="s">
         <v>108</v>
       </c>
@@ -2033,7 +2072,7 @@
       </c>
       <c r="F43" s="32"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="35" t="s">
         <v>110</v>
       </c>
@@ -2051,7 +2090,7 @@
       </c>
       <c r="F44" s="32"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
         <v>111</v>
       </c>
@@ -2069,7 +2108,7 @@
       </c>
       <c r="F45" s="32"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="31"/>
       <c r="B46" s="31" t="s">
         <v>72</v>
@@ -2085,7 +2124,7 @@
       </c>
       <c r="F46" s="28"/>
     </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="35" t="s">
         <v>113</v>
       </c>
@@ -2105,7 +2144,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="s">
         <v>114</v>
       </c>
@@ -2123,7 +2162,7 @@
       </c>
       <c r="F48" s="32"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="35" t="s">
         <v>115</v>
       </c>
@@ -2141,7 +2180,7 @@
       </c>
       <c r="F49" s="32"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="35" t="s">
         <v>116</v>
       </c>
@@ -2159,7 +2198,7 @@
       </c>
       <c r="F50" s="32"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="35" t="s">
         <v>117</v>
       </c>
@@ -2177,7 +2216,7 @@
       </c>
       <c r="F51" s="32"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="35" t="s">
         <v>42</v>
       </c>
@@ -2195,7 +2234,7 @@
       </c>
       <c r="F52" s="32"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="39" t="s">
         <v>118</v>
       </c>
@@ -2213,7 +2252,7 @@
       </c>
       <c r="F53" s="36"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="39" t="s">
         <v>119</v>
       </c>
@@ -2231,7 +2270,7 @@
       </c>
       <c r="F54" s="36"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="39" t="s">
         <v>120</v>
       </c>
@@ -2249,7 +2288,7 @@
       </c>
       <c r="F55" s="36"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="39" t="s">
         <v>123</v>
       </c>
@@ -2267,7 +2306,7 @@
       </c>
       <c r="F56" s="36"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="39" t="s">
         <v>124</v>
       </c>
@@ -2285,7 +2324,7 @@
       </c>
       <c r="F57" s="36"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="39" t="s">
         <v>109</v>
       </c>
@@ -2305,7 +2344,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="39" t="s">
         <v>125</v>
       </c>
@@ -2323,7 +2362,7 @@
       </c>
       <c r="F59" s="36"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="39" t="s">
         <v>45</v>
       </c>
@@ -2341,7 +2380,7 @@
       </c>
       <c r="F60" s="36"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="39" t="s">
         <v>126</v>
       </c>
@@ -2359,7 +2398,7 @@
       </c>
       <c r="F61" s="36"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="39" t="s">
         <v>127</v>
       </c>
@@ -2377,7 +2416,7 @@
       </c>
       <c r="F62" s="36"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="39" t="s">
         <v>128</v>
       </c>
@@ -2395,7 +2434,7 @@
       </c>
       <c r="F63" s="36"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="39" t="s">
         <v>129</v>
       </c>
@@ -2415,7 +2454,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="39" t="s">
         <v>153</v>
       </c>
@@ -2433,7 +2472,7 @@
       </c>
       <c r="F65" s="36"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="39" t="s">
         <v>154</v>
       </c>
@@ -2451,7 +2490,7 @@
       </c>
       <c r="F66" s="36"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="39" t="s">
         <v>156</v>
       </c>
@@ -2469,7 +2508,7 @@
       </c>
       <c r="F67" s="36"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="39" t="s">
         <v>157</v>
       </c>
@@ -2487,7 +2526,7 @@
       </c>
       <c r="F68" s="36"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="39" t="s">
         <v>171</v>
       </c>
@@ -2505,7 +2544,7 @@
       </c>
       <c r="F69" s="36"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="39" t="s">
         <v>182</v>
       </c>
@@ -2523,91 +2562,89 @@
       </c>
       <c r="F70" s="36"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="27" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="52" t="s">
+        <v>203</v>
+      </c>
+      <c r="B71" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" s="37">
+        <v>619</v>
+      </c>
+      <c r="D71" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="F71" s="36"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="27" t="s">
         <v>130</v>
-      </c>
-      <c r="B71" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C71" s="25">
-        <v>701</v>
-      </c>
-      <c r="D71" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E71" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="F71" s="24"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="27" t="s">
-        <v>121</v>
       </c>
       <c r="B72" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C72" s="25">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D72" s="26" t="s">
         <v>66</v>
       </c>
       <c r="E72" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F72" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="F72" s="24"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="27" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B73" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C73" s="25">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D73" s="26" t="s">
         <v>66</v>
       </c>
       <c r="E73" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F73" s="24"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B74" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C74" s="25">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E74" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F74" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="F74" s="24"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B75" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C75" s="25">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D75" s="26" t="s">
         <v>0</v>
@@ -2619,15 +2656,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B76" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C76" s="25">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D76" s="26" t="s">
         <v>0</v>
@@ -2636,18 +2673,18 @@
         <v>12</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B77" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C77" s="25">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D77" s="26" t="s">
         <v>0</v>
@@ -2659,15 +2696,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B78" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C78" s="25">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D78" s="26" t="s">
         <v>0</v>
@@ -2676,18 +2713,18 @@
         <v>12</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B79" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C79" s="25">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D79" s="26" t="s">
         <v>0</v>
@@ -2699,555 +2736,575 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B80" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C80" s="25">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D80" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F80" s="24"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B81" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C81" s="25">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D81" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E81" s="27" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F81" s="24"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="27" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
       <c r="B82" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C82" s="25">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D82" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E82" s="27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F82" s="24"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="27" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="B83" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C83" s="25">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D83" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F83" s="24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="F83" s="24"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B84" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C84" s="25">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D84" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E84" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="F84" s="24"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="F84" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B85" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C85" s="25">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D85" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>52</v>
+        <v>173</v>
       </c>
       <c r="F85" s="24"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B86" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C86" s="25">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D86" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E86" s="27" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="F86" s="24"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="27" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="B87" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C87" s="25">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D87" s="26" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="E87" s="27" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F87" s="24"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="27" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="B88" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C88" s="25">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D88" s="26" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E88" s="27" t="s">
-        <v>184</v>
+        <v>31</v>
       </c>
       <c r="F88" s="24"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="27" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B89" s="27" t="s">
         <v>74</v>
       </c>
       <c r="C89" s="25">
+        <v>718</v>
+      </c>
+      <c r="D89" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="F89" s="24"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="B90" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C90" s="25">
         <v>719</v>
       </c>
-      <c r="D89" s="26" t="s">
+      <c r="D90" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="E89" s="27" t="s">
+      <c r="E90" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="F89" s="24"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="43" t="s">
+      <c r="F90" s="24"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="43" t="s">
         <v>9</v>
-      </c>
-      <c r="B90" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C90" s="41">
-        <v>801</v>
-      </c>
-      <c r="D90" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E90" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="F90" s="40"/>
-    </row>
-    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="43" t="s">
-        <v>44</v>
       </c>
       <c r="B91" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C91" s="41">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D91" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E91" s="43" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="F91" s="40"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A92" s="43" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B92" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C92" s="41">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D92" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E92" s="43" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="F92" s="40"/>
     </row>
-    <row r="93" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B93" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C93" s="41">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D93" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E93" s="43" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="F93" s="40"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A94" s="43" t="s">
-        <v>144</v>
+        <v>49</v>
       </c>
       <c r="B94" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C94" s="41">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D94" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E94" s="43" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F94" s="40"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="43" t="s">
-        <v>53</v>
+        <v>144</v>
       </c>
       <c r="B95" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C95" s="41">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D95" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E95" s="43" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F95" s="40"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B96" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C96" s="41">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D96" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E96" s="43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F96" s="40"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="43" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="B97" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C97" s="41">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D97" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E97" s="43" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F97" s="40"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="43" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="B98" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C98" s="41">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D98" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E98" s="43" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="F98" s="40"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="43" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B99" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C99" s="41">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D99" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E99" s="43" t="s">
-        <v>165</v>
+        <v>50</v>
       </c>
       <c r="F99" s="40"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B100" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C100" s="41">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D100" s="42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" s="43" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F100" s="40"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B101" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C101" s="41">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D101" s="42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E101" s="43" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F101" s="40"/>
     </row>
-    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="43" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B102" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C102" s="41">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D102" s="42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102" s="43" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F102" s="40"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A103" s="43" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B103" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C103" s="41">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D103" s="42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" s="43" t="s">
-        <v>20</v>
+        <v>175</v>
       </c>
       <c r="F103" s="40"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="43" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B104" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C104" s="41">
+        <v>814</v>
+      </c>
+      <c r="D104" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F104" s="40"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="B105" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="C105" s="41">
         <v>815</v>
       </c>
-      <c r="D104" s="42" t="s">
+      <c r="D105" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E104" s="43" t="s">
+      <c r="E105" s="43" t="s">
         <v>199</v>
       </c>
-      <c r="F104" s="40"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="47" t="s">
+      <c r="F105" s="40"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="47" t="s">
         <v>30</v>
-      </c>
-      <c r="B105" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C105" s="45">
-        <v>901</v>
-      </c>
-      <c r="D105" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E105" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="F105" s="44"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="47" t="s">
-        <v>150</v>
       </c>
       <c r="B106" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C106" s="45">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D106" s="46" t="s">
         <v>66</v>
       </c>
       <c r="E106" s="47" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F106" s="44"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="47" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B107" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C107" s="45">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D107" s="46" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E107" s="47" t="s">
-        <v>29</v>
+        <v>151</v>
       </c>
       <c r="F107" s="44"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B108" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C108" s="45">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D108" s="46" t="s">
-        <v>66</v>
+        <v>0</v>
       </c>
       <c r="E108" s="47" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F108" s="44"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="47" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B109" s="47" t="s">
         <v>73</v>
       </c>
       <c r="C109" s="45">
+        <v>904</v>
+      </c>
+      <c r="D109" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E109" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="F109" s="44"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="B110" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C110" s="45">
         <v>905</v>
       </c>
-      <c r="D109" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E109" s="47" t="s">
+      <c r="D110" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="F109" s="44"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="2"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="3"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="2"/>
-      <c r="F110" s="1"/>
+      <c r="F110" s="44"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="2"/>
+      <c r="F111" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:E69">

</xml_diff>

<commit_message>
Update README, classifiers, NetworkConnection and initial Data Markings.
</commit_message>
<xml_diff>
--- a/elevator_log_messages.xlsx
+++ b/elevator_log_messages.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpiazza/git/cti-stix-elevator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmanuelle\PycharmProjects\cti-stix-elevator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="11500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="19200" windowHeight="11505" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Error Codes - STIX Elevator" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="207">
   <si>
     <t>warn</t>
   </si>
@@ -53,12 +53,6 @@
     <t>process_description_and_short_description</t>
   </si>
   <si>
-    <t>finish_basic_object</t>
-  </si>
-  <si>
-    <t>Handling not implemented, yet</t>
-  </si>
-  <si>
     <t>add_string_property_to_description</t>
   </si>
   <si>
@@ -639,12 +633,27 @@
   </si>
   <si>
     <t>No start time for the first valid time interval is available in %s, other time intervals might be more appropriate</t>
+  </si>
+  <si>
+    <t>[xxx] content is not supported in STIX 2.0</t>
+  </si>
+  <si>
+    <t>convert_network_connection</t>
+  </si>
+  <si>
+    <t>Only one Layer7_Connections/HTTP_Request_Response used fot http-request-ext, using first value</t>
+  </si>
+  <si>
+    <t>Could not resolve Marking Structure [id]</t>
+  </si>
+  <si>
+    <t>convert_marking_specification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -846,7 +855,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -964,6 +973,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="31" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="31"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="20% - Accent2" xfId="31" builtinId="34"/>
@@ -1282,34 +1292,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="77.1640625" style="23" customWidth="1"/>
+    <col min="1" max="1" width="77.125" style="23" customWidth="1"/>
     <col min="2" max="2" width="49" style="23" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="40.1640625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="7.625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="7.625" customWidth="1"/>
+    <col min="5" max="5" width="40.125" style="23" customWidth="1"/>
     <col min="6" max="6" width="65.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>3</v>
@@ -1318,7 +1328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="9"/>
@@ -1326,12 +1336,12 @@
       <c r="E2" s="20"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C3" s="11">
         <v>201</v>
@@ -1340,18 +1350,18 @@
         <v>0</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C4" s="11">
         <v>202</v>
@@ -1360,16 +1370,16 @@
         <v>1</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C5" s="11">
         <v>203</v>
@@ -1378,34 +1388,34 @@
         <v>1</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C6" s="11">
         <v>204</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C7" s="11">
         <v>205</v>
@@ -1414,16 +1424,16 @@
         <v>0</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C8" s="11">
         <v>206</v>
@@ -1432,16 +1442,16 @@
         <v>0</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C9" s="11">
         <v>207</v>
@@ -1450,16 +1460,16 @@
         <v>1</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C10" s="11">
         <v>208</v>
@@ -1468,18 +1478,18 @@
         <v>0</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" s="11">
         <v>209</v>
@@ -1488,16 +1498,16 @@
         <v>0</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" s="11">
         <v>210</v>
@@ -1506,16 +1516,16 @@
         <v>1</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="15">
         <v>301</v>
@@ -1530,12 +1540,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C14" s="15">
         <v>302</v>
@@ -1544,34 +1554,34 @@
         <v>0</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C15" s="15">
         <v>303</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="15">
         <v>304</v>
@@ -1580,16 +1590,16 @@
         <v>0</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="15">
         <v>305</v>
@@ -1598,16 +1608,16 @@
         <v>0</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="15">
         <v>306</v>
@@ -1616,16 +1626,16 @@
         <v>0</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C19" s="18">
         <v>401</v>
@@ -1638,12 +1648,12 @@
       </c>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C20" s="18">
         <v>402</v>
@@ -1652,16 +1662,16 @@
         <v>0</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F20" s="17"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" s="18">
         <v>403</v>
@@ -1670,18 +1680,18 @@
         <v>0</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C22" s="18">
         <v>404</v>
@@ -1690,18 +1700,18 @@
         <v>0</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" s="18">
         <v>405</v>
@@ -1710,16 +1720,16 @@
         <v>0</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C24" s="18">
         <v>406</v>
@@ -1728,16 +1738,16 @@
         <v>0</v>
       </c>
       <c r="E24" s="22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C25" s="18">
         <v>407</v>
@@ -1746,16 +1756,16 @@
         <v>0</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F25" s="17"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C26" s="18">
         <v>408</v>
@@ -1764,16 +1774,16 @@
         <v>0</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C27" s="18">
         <v>409</v>
@@ -1782,16 +1792,16 @@
         <v>0</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F27" s="17"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C28" s="18">
         <v>410</v>
@@ -1800,16 +1810,16 @@
         <v>0</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C29" s="18">
         <v>411</v>
@@ -1818,16 +1828,16 @@
         <v>0</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C30" s="18">
         <v>412</v>
@@ -1836,16 +1846,16 @@
         <v>0</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C31" s="18">
         <v>413</v>
@@ -1854,16 +1864,16 @@
         <v>0</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C32" s="18">
         <v>414</v>
@@ -1872,16 +1882,16 @@
         <v>0</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F32" s="17"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C33" s="18">
         <v>415</v>
@@ -1890,16 +1900,16 @@
         <v>0</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C34" s="18">
         <v>416</v>
@@ -1908,16 +1918,16 @@
         <v>0</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C35" s="18">
         <v>417</v>
@@ -1926,16 +1936,16 @@
         <v>0</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" s="18">
         <v>418</v>
@@ -1944,16 +1954,16 @@
         <v>0</v>
       </c>
       <c r="E36" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="17"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F36" s="17"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="22" t="s">
-        <v>58</v>
-      </c>
       <c r="B37" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C37" s="18">
         <v>419</v>
@@ -1962,16 +1972,16 @@
         <v>0</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38" s="18">
         <v>420</v>
@@ -1980,16 +1990,16 @@
         <v>0</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C39" s="18">
         <v>421</v>
@@ -1998,16 +2008,16 @@
         <v>0</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C40" s="18">
         <v>422</v>
@@ -2016,16 +2026,16 @@
         <v>0</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="49" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C41" s="18">
         <v>423</v>
@@ -2034,1277 +2044,1313 @@
         <v>0</v>
       </c>
       <c r="E41" s="50" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="31"/>
-      <c r="B42" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="29">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="18">
+        <v>424</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="F42" s="17"/>
+    </row>
+    <row r="43" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
+      <c r="B43" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="29">
         <v>501</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D43" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E42" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="28"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="35" t="s">
+      <c r="E43" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="28"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="33">
+        <v>502</v>
+      </c>
+      <c r="D44" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F44" s="32"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="B43" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C43" s="33">
-        <v>502</v>
-      </c>
-      <c r="D43" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="F43" s="32"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" s="33">
+      <c r="B45" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="33">
         <v>503</v>
       </c>
-      <c r="D44" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="F44" s="32"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="35" t="s">
+      <c r="D45" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" s="32"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="33">
+        <v>504</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="32"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="31"/>
+      <c r="B47" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="29">
+        <v>505</v>
+      </c>
+      <c r="D47" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" s="28"/>
+    </row>
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B45" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="33">
-        <v>504</v>
-      </c>
-      <c r="D45" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="35" t="s">
+      <c r="B48" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="33">
+        <v>506</v>
+      </c>
+      <c r="D48" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C49" s="33">
+        <v>507</v>
+      </c>
+      <c r="D49" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F45" s="32"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" s="29">
-        <v>505</v>
-      </c>
-      <c r="D46" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="F46" s="28"/>
-    </row>
-    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A47" s="35" t="s">
+      <c r="F49" s="32"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="B47" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C47" s="33">
-        <v>506</v>
-      </c>
-      <c r="D47" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E47" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="F47" s="32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="35" t="s">
+      <c r="B50" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="33">
+        <v>508</v>
+      </c>
+      <c r="D50" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="F50" s="32"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="B48" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C48" s="33">
-        <v>507</v>
-      </c>
-      <c r="D48" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F48" s="32"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="35" t="s">
+      <c r="B51" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="33">
+        <v>509</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="F51" s="32"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="B49" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C49" s="33">
-        <v>508</v>
-      </c>
-      <c r="D49" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F49" s="32"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="35" t="s">
+      <c r="B52" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="33">
+        <v>510</v>
+      </c>
+      <c r="D52" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="F52" s="32"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="33">
+        <v>511</v>
+      </c>
+      <c r="D53" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E53" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F53" s="32"/>
+    </row>
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="33">
+        <v>512</v>
+      </c>
+      <c r="D54" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="F54" s="32"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="B50" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C50" s="33">
-        <v>509</v>
-      </c>
-      <c r="D50" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E50" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="F50" s="32"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="35" t="s">
+      <c r="B55" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C55" s="37">
+        <v>601</v>
+      </c>
+      <c r="D55" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="36"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" s="33">
-        <v>510</v>
-      </c>
-      <c r="D51" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E51" s="35" t="s">
-        <v>64</v>
-      </c>
-      <c r="F51" s="32"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C52" s="33">
-        <v>511</v>
-      </c>
-      <c r="D52" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="E52" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="F52" s="32"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="39" t="s">
+      <c r="B56" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C56" s="37">
+        <v>602</v>
+      </c>
+      <c r="D56" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="36"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="B53" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C53" s="37">
-        <v>601</v>
-      </c>
-      <c r="D53" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="F53" s="36"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="B54" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C54" s="37">
-        <v>602</v>
-      </c>
-      <c r="D54" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="F54" s="36"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="B55" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" s="37">
+      <c r="B57" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="37">
         <v>603</v>
       </c>
-      <c r="D55" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F55" s="36"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="B56" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C56" s="37">
+      <c r="D57" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="F57" s="36"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" s="37">
         <v>604</v>
-      </c>
-      <c r="D56" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="E56" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="F56" s="36"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="B57" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C57" s="37">
-        <v>605</v>
-      </c>
-      <c r="D57" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E57" s="39" t="s">
-        <v>122</v>
-      </c>
-      <c r="F57" s="36"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="B58" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" s="37">
-        <v>606</v>
       </c>
       <c r="D58" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E58" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="F58" s="36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="F58" s="36"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C59" s="37">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59" s="39" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="F59" s="36"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="39" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C60" s="37">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D60" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E60" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="F60" s="36"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="F60" s="36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="39" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C61" s="37">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D61" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F61" s="36"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="39" t="s">
-        <v>127</v>
+        <v>43</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C62" s="37">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" s="39" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="F62" s="36"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="39" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C63" s="37">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D63" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E63" s="39" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F63" s="36"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" s="37">
+        <v>610</v>
+      </c>
+      <c r="D64" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F64" s="36"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C65" s="37">
+        <v>611</v>
+      </c>
+      <c r="D65" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F65" s="36"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B66" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C66" s="37">
+        <v>612</v>
+      </c>
+      <c r="D66" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E66" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F66" s="36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67" s="37">
+        <v>613</v>
+      </c>
+      <c r="D67" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="F67" s="36"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="B68" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="37">
+        <v>614</v>
+      </c>
+      <c r="D68" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E68" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="F68" s="36"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B69" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C69" s="37">
+        <v>615</v>
+      </c>
+      <c r="D69" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E69" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="F69" s="36"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B70" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" s="37">
+        <v>616</v>
+      </c>
+      <c r="D70" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E70" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="F70" s="36"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="B71" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C71" s="37">
+        <v>617</v>
+      </c>
+      <c r="D71" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="39" t="s">
+        <v>170</v>
+      </c>
+      <c r="F71" s="36"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B72" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C72" s="37">
+        <v>618</v>
+      </c>
+      <c r="D72" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E72" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="F72" s="36"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="52" t="s">
+        <v>201</v>
+      </c>
+      <c r="B73" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C73" s="37">
+        <v>619</v>
+      </c>
+      <c r="D73" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F73" s="36"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B74" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74" s="25">
+        <v>701</v>
+      </c>
+      <c r="D74" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E74" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F74" s="24"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" s="25">
+        <v>702</v>
+      </c>
+      <c r="D75" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F75" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="B64" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C64" s="37">
-        <v>612</v>
-      </c>
-      <c r="D64" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="E64" s="39" t="s">
+      <c r="B76" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76" s="25">
+        <v>703</v>
+      </c>
+      <c r="D76" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E76" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F76" s="24"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B77" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C77" s="25">
+        <v>704</v>
+      </c>
+      <c r="D77" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B78" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C78" s="25">
+        <v>705</v>
+      </c>
+      <c r="D78" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B79" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C79" s="25">
+        <v>706</v>
+      </c>
+      <c r="D79" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="B80" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C80" s="25">
+        <v>707</v>
+      </c>
+      <c r="D80" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B81" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C81" s="25">
+        <v>708</v>
+      </c>
+      <c r="D81" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E81" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B82" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C82" s="25">
+        <v>709</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B83" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C83" s="25">
+        <v>710</v>
+      </c>
+      <c r="D83" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F83" s="24"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="B84" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C84" s="25">
+        <v>711</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F84" s="24"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B85" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C85" s="25">
+        <v>712</v>
+      </c>
+      <c r="D85" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F64" s="36" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="B65" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" s="37">
-        <v>613</v>
-      </c>
-      <c r="D65" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="F65" s="36"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="39" t="s">
-        <v>154</v>
-      </c>
-      <c r="B66" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C66" s="37">
-        <v>614</v>
-      </c>
-      <c r="D66" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="39" t="s">
-        <v>152</v>
-      </c>
-      <c r="F66" s="36"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="39" t="s">
-        <v>156</v>
-      </c>
-      <c r="B67" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C67" s="37">
-        <v>615</v>
-      </c>
-      <c r="D67" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E67" s="39" t="s">
+      <c r="F85" s="24"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B86" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C86" s="25">
+        <v>713</v>
+      </c>
+      <c r="D86" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F86" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="B87" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C87" s="25">
+        <v>714</v>
+      </c>
+      <c r="D87" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="F87" s="24"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C88" s="25">
+        <v>715</v>
+      </c>
+      <c r="D88" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F88" s="24"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="B89" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C89" s="25">
+        <v>716</v>
+      </c>
+      <c r="D89" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F89" s="24"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="F67" s="36"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="B68" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C68" s="37">
-        <v>616</v>
-      </c>
-      <c r="D68" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E68" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="F68" s="36"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="39" t="s">
-        <v>171</v>
-      </c>
-      <c r="B69" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C69" s="37">
-        <v>617</v>
-      </c>
-      <c r="D69" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E69" s="39" t="s">
-        <v>172</v>
-      </c>
-      <c r="F69" s="36"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="39" t="s">
+      <c r="B90" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C90" s="25">
+        <v>717</v>
+      </c>
+      <c r="D90" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E90" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F90" s="24"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="B91" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C91" s="25">
+        <v>718</v>
+      </c>
+      <c r="D91" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="B70" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C70" s="37">
-        <v>618</v>
-      </c>
-      <c r="D70" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E70" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="F70" s="36"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="52" t="s">
-        <v>203</v>
-      </c>
-      <c r="B71" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="C71" s="37">
-        <v>619</v>
-      </c>
-      <c r="D71" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E71" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="F71" s="36"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B72" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C72" s="25">
-        <v>701</v>
-      </c>
-      <c r="D72" s="26" t="s">
+      <c r="F91" s="24"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="B92" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C92" s="25">
+        <v>719</v>
+      </c>
+      <c r="D92" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E92" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="F92" s="24"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="43" t="s">
+        <v>205</v>
+      </c>
+      <c r="B93" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E72" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="F72" s="24"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="B73" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C73" s="25">
-        <v>702</v>
-      </c>
-      <c r="D73" s="26" t="s">
+      <c r="C93" s="41">
+        <v>801</v>
+      </c>
+      <c r="D93" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="43" t="s">
+        <v>206</v>
+      </c>
+      <c r="F93" s="40"/>
+    </row>
+    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B94" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E73" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F73" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B74" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C74" s="25">
-        <v>703</v>
-      </c>
-      <c r="D74" s="26" t="s">
+      <c r="C94" s="41">
+        <v>802</v>
+      </c>
+      <c r="D94" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="F94" s="40"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B95" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E74" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F74" s="24"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B75" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C75" s="25">
-        <v>704</v>
-      </c>
-      <c r="D75" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E75" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F75" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="B76" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C76" s="25">
-        <v>705</v>
-      </c>
-      <c r="D76" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E76" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F76" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B77" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" s="25">
-        <v>706</v>
-      </c>
-      <c r="D77" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E77" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F77" s="24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="B78" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C78" s="25">
-        <v>707</v>
-      </c>
-      <c r="D78" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E78" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F78" s="24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="B79" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C79" s="25">
-        <v>708</v>
-      </c>
-      <c r="D79" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E79" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F79" s="24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="B80" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C80" s="25">
-        <v>709</v>
-      </c>
-      <c r="D80" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E80" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F80" s="24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="B81" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C81" s="25">
-        <v>710</v>
-      </c>
-      <c r="D81" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="F81" s="24"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="B82" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C82" s="25">
-        <v>711</v>
-      </c>
-      <c r="D82" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E82" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="F82" s="24"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="B83" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C83" s="25">
-        <v>712</v>
-      </c>
-      <c r="D83" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E83" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F83" s="24"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="B84" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C84" s="25">
-        <v>713</v>
-      </c>
-      <c r="D84" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F84" s="24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="B85" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C85" s="25">
-        <v>714</v>
-      </c>
-      <c r="D85" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E85" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="F85" s="24"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="27" t="s">
+      <c r="C95" s="41">
+        <v>803</v>
+      </c>
+      <c r="D95" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F95" s="40"/>
+    </row>
+    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B96" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C96" s="41">
+        <v>804</v>
+      </c>
+      <c r="D96" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F96" s="40"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="B86" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C86" s="25">
-        <v>715</v>
-      </c>
-      <c r="D86" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E86" s="27" t="s">
+      <c r="B97" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C97" s="41">
+        <v>805</v>
+      </c>
+      <c r="D97" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="F97" s="40"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B98" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C98" s="41">
+        <v>806</v>
+      </c>
+      <c r="D98" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="F86" s="24"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="27" t="s">
+      <c r="F98" s="40"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B99" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C99" s="41">
+        <v>807</v>
+      </c>
+      <c r="D99" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="F99" s="40"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="B87" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C87" s="25">
-        <v>716</v>
-      </c>
-      <c r="D87" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E87" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="F87" s="24"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="B88" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C88" s="25">
-        <v>717</v>
-      </c>
-      <c r="D88" s="26" t="s">
+      <c r="B100" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E88" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="F88" s="24"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="B89" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C89" s="25">
-        <v>718</v>
-      </c>
-      <c r="D89" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E89" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="F89" s="24"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="B90" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="C90" s="25">
-        <v>719</v>
-      </c>
-      <c r="D90" s="26" t="s">
+      <c r="C100" s="41">
+        <v>808</v>
+      </c>
+      <c r="D100" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="F100" s="40"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="B101" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E90" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="F90" s="24"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="B91" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C91" s="41">
-        <v>801</v>
-      </c>
-      <c r="D91" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E91" s="43" t="s">
-        <v>8</v>
-      </c>
-      <c r="F91" s="40"/>
-    </row>
-    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A92" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B92" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C92" s="41">
-        <v>802</v>
-      </c>
-      <c r="D92" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E92" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="F92" s="40"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B93" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C93" s="41">
-        <v>803</v>
-      </c>
-      <c r="D93" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E93" s="43" t="s">
+      <c r="C101" s="41">
+        <v>809</v>
+      </c>
+      <c r="D101" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E101" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="F93" s="40"/>
-    </row>
-    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A94" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="B94" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C94" s="41">
-        <v>804</v>
-      </c>
-      <c r="D94" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E94" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="F94" s="40"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="43" t="s">
-        <v>144</v>
-      </c>
-      <c r="B95" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C95" s="41">
-        <v>805</v>
-      </c>
-      <c r="D95" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E95" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="F95" s="40"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B96" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C96" s="41">
-        <v>806</v>
-      </c>
-      <c r="D96" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E96" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="F96" s="40"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="B97" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C97" s="41">
-        <v>807</v>
-      </c>
-      <c r="D97" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="F97" s="40"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="43" t="s">
-        <v>145</v>
-      </c>
-      <c r="B98" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C98" s="41">
-        <v>808</v>
-      </c>
-      <c r="D98" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E98" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="F98" s="40"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="43" t="s">
-        <v>161</v>
-      </c>
-      <c r="B99" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C99" s="41">
-        <v>809</v>
-      </c>
-      <c r="D99" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E99" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="F99" s="40"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="43" t="s">
-        <v>164</v>
-      </c>
-      <c r="B100" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C100" s="41">
+      <c r="F101" s="40"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="B102" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C102" s="41">
         <v>810</v>
       </c>
-      <c r="D100" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E100" s="43" t="s">
+      <c r="D102" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="F102" s="40"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="F100" s="40"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="43" t="s">
-        <v>167</v>
-      </c>
-      <c r="B101" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C101" s="41">
+      <c r="B103" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C103" s="41">
         <v>811</v>
-      </c>
-      <c r="D101" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="E101" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="F101" s="40"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="43" t="s">
-        <v>169</v>
-      </c>
-      <c r="B102" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C102" s="41">
-        <v>812</v>
-      </c>
-      <c r="D102" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E102" s="43" t="s">
-        <v>170</v>
-      </c>
-      <c r="F102" s="40"/>
-    </row>
-    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A103" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="B103" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C103" s="41">
-        <v>813</v>
       </c>
       <c r="D103" s="42" t="s">
         <v>1</v>
       </c>
       <c r="E103" s="43" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F103" s="40"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="43" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="B104" s="43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C104" s="41">
+        <v>812</v>
+      </c>
+      <c r="D104" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="F104" s="40"/>
+    </row>
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="B105" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C105" s="41">
+        <v>813</v>
+      </c>
+      <c r="D105" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E105" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="F105" s="40"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="B106" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C106" s="41">
         <v>814</v>
       </c>
-      <c r="D104" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E104" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="F104" s="40"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="43" t="s">
-        <v>198</v>
-      </c>
-      <c r="B105" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C105" s="41">
+      <c r="D106" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F106" s="40"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="B107" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C107" s="41">
         <v>815</v>
       </c>
-      <c r="D105" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="E105" s="43" t="s">
-        <v>199</v>
-      </c>
-      <c r="F105" s="40"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="B106" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C106" s="45">
+      <c r="D107" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E107" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="F107" s="40"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B108" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C108" s="45">
         <v>901</v>
       </c>
-      <c r="D106" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E106" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="F106" s="44"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="47" t="s">
-        <v>150</v>
-      </c>
-      <c r="B107" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C107" s="45">
+      <c r="D108" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E108" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="F108" s="44"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="B109" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C109" s="45">
         <v>902</v>
       </c>
-      <c r="D107" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E107" s="47" t="s">
-        <v>151</v>
-      </c>
-      <c r="F107" s="44"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="B108" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C108" s="45">
-        <v>903</v>
-      </c>
-      <c r="D108" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E108" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="F108" s="44"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="47" t="s">
+      <c r="D109" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E109" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="B109" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C109" s="45">
-        <v>904</v>
-      </c>
-      <c r="D109" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="E109" s="47" t="s">
-        <v>34</v>
-      </c>
       <c r="F109" s="44"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="47" t="s">
         <v>146</v>
       </c>
       <c r="B110" s="47" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C110" s="45">
+        <v>903</v>
+      </c>
+      <c r="D110" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F110" s="44"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="B111" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C111" s="45">
+        <v>904</v>
+      </c>
+      <c r="D111" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E111" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="F111" s="44"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="B112" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C112" s="45">
         <v>905</v>
       </c>
-      <c r="D110" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E110" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="F110" s="44"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" s="2"/>
-      <c r="B111" s="2"/>
-      <c r="C111" s="3"/>
-      <c r="D111" s="1"/>
-      <c r="E111" s="2"/>
-      <c r="F111" s="1"/>
+      <c r="D112" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="F112" s="44"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:E69">

</xml_diff>

<commit_message>
keep track of object id to pattern mapping handle email attachments make sure strings are put into the json, not objects handle email cc and bcc handle related objects in certain cases (email attachments) collapse references into one pattern handle placeholders are rhs of comparison expressions lookup placeholders via object ids handle expressions missing the rhs because the xml element is empty strip whitespace for rhs replace : when . should be used handle None returnbed from add_comparison_expression handle file name extensions handle redundant reg hive and reg key values fix import of stix package depending upon version insure that a message is printed for every relationship which is missing a source or target ref handle cybox relationships make globals in ids.py be local to the file create logger even if no message_log_directory option
</commit_message>
<xml_diff>
--- a/elevator_log_messages.xlsx
+++ b/elevator_log_messages.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmanuelle\PycharmProjects\cti-stix-elevator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpiazza/git/cti-stix-elevator/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="19200" windowHeight="11505" tabRatio="500"/>
+    <workbookView xWindow="32120" yWindow="-12900" windowWidth="24360" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Error Codes - STIX Elevator" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="213">
   <si>
     <t>warn</t>
   </si>
@@ -182,9 +182,6 @@
     <t>create_term</t>
   </si>
   <si>
-    <t>Email attachments not handled yet</t>
-  </si>
-  <si>
     <t>convert_email_message_to_pattern</t>
   </si>
   <si>
@@ -311,9 +308,6 @@
     <t>ExploitTarget/Configurations type in [id] not supported in STIX 2.0</t>
   </si>
   <si>
-    <t>Indicator [id] has an observable or indicator composite expression which is not supported in STIX 2.0</t>
-  </si>
-  <si>
     <t>TTP/Behavior/Exploits/Exploit in [id] not supported in STIX 2.0</t>
   </si>
   <si>
@@ -521,9 +515,6 @@
     <t>convert_indicator_to_pattern</t>
   </si>
   <si>
-    <t>No term was yielded for [id]</t>
-  </si>
-  <si>
     <t>Network Connection not implemented, yet.</t>
   </si>
   <si>
@@ -648,13 +639,47 @@
   </si>
   <si>
     <t>convert_marking_specification</t>
+  </si>
+  <si>
+    <t>Unable to create a pattern from a File object</t>
+  </si>
+  <si>
+    <t>convert_file_name_and_path_to_pattern</t>
+  </si>
+  <si>
+    <t>[stix 1.x property] contains no value</t>
+  </si>
+  <si>
+    <t>No pattern term was created from [id]</t>
+  </si>
+  <si>
+    <t>Email [property] not handled yet</t>
+  </si>
+  <si>
+    <t>various</t>
+  </si>
+  <si>
+    <t>No term was yielded for %s</t>
+  </si>
+  <si>
+    <t>Hive property, %s, is already a prefix of the key property, %s</t>
+  </si>
+  <si>
+    <t>Indicator %s has an observable or indicator composite expression which may not supported correctly in STIX 2.0 - please check this pattern</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -708,6 +733,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -780,7 +812,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -818,164 +850,205 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="34">
+  <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="31" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="31"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="31" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="31" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="31" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="31" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="31" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="31" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="34">
+  <cellStyles count="56">
     <cellStyle name="20% - Accent2" xfId="31" builtinId="34"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -993,6 +1066,17 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1009,6 +1093,17 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1292,34 +1387,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:F117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="77.125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="77.1640625" style="23" customWidth="1"/>
     <col min="2" max="2" width="49" style="23" customWidth="1"/>
-    <col min="3" max="3" width="7.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="7.625" customWidth="1"/>
-    <col min="5" max="5" width="40.125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" style="23" customWidth="1"/>
     <col min="6" max="6" width="65.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>74</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>75</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>3</v>
@@ -1328,7 +1423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="9"/>
@@ -1336,12 +1431,12 @@
       <c r="E2" s="20"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="21" t="s">
         <v>79</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>80</v>
       </c>
       <c r="C3" s="11">
         <v>201</v>
@@ -1350,18 +1445,18 @@
         <v>0</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C4" s="11">
         <v>202</v>
@@ -1370,16 +1465,16 @@
         <v>1</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="11">
         <v>203</v>
@@ -1388,34 +1483,34 @@
         <v>1</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" s="11">
         <v>204</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" s="11">
         <v>205</v>
@@ -1428,12 +1523,12 @@
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="11">
         <v>206</v>
@@ -1446,12 +1541,12 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="11">
         <v>207</v>
@@ -1460,16 +1555,16 @@
         <v>1</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="11">
         <v>208</v>
@@ -1481,15 +1576,15 @@
         <v>38</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="11">
         <v>209</v>
@@ -1498,16 +1593,16 @@
         <v>0</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="11">
         <v>210</v>
@@ -1516,16 +1611,16 @@
         <v>1</v>
       </c>
       <c r="E12" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>82</v>
-      </c>
       <c r="B13" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="15">
         <v>301</v>
@@ -1540,12 +1635,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="15">
         <v>302</v>
@@ -1558,30 +1653,30 @@
       </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" s="15">
         <v>303</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="15">
         <v>304</v>
@@ -1590,16 +1685,16 @@
         <v>0</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="15">
         <v>305</v>
@@ -1608,16 +1703,16 @@
         <v>0</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="15">
         <v>306</v>
@@ -1626,16 +1721,16 @@
         <v>0</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="18">
         <v>401</v>
@@ -1648,12 +1743,12 @@
       </c>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="18">
         <v>402</v>
@@ -1662,16 +1757,16 @@
         <v>0</v>
       </c>
       <c r="E20" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="17"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>67</v>
-      </c>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>68</v>
       </c>
       <c r="C21" s="18">
         <v>403</v>
@@ -1686,12 +1781,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="18">
         <v>404</v>
@@ -1706,12 +1801,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="18">
         <v>405</v>
@@ -1724,12 +1819,12 @@
       </c>
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="18">
         <v>406</v>
@@ -1742,12 +1837,12 @@
       </c>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
-        <v>94</v>
+        <v>212</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="18">
         <v>407</v>
@@ -1760,12 +1855,12 @@
       </c>
       <c r="F25" s="17"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="18">
         <v>408</v>
@@ -1778,12 +1873,12 @@
       </c>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="18">
         <v>409</v>
@@ -1796,12 +1891,12 @@
       </c>
       <c r="F27" s="17"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="18">
         <v>410</v>
@@ -1814,12 +1909,12 @@
       </c>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="18">
         <v>411</v>
@@ -1832,12 +1927,12 @@
       </c>
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="18">
         <v>412</v>
@@ -1850,12 +1945,12 @@
       </c>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="18">
         <v>413</v>
@@ -1868,12 +1963,12 @@
       </c>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="18">
         <v>414</v>
@@ -1886,12 +1981,12 @@
       </c>
       <c r="F32" s="17"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="18">
         <v>415</v>
@@ -1904,12 +1999,12 @@
       </c>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="18">
         <v>416</v>
@@ -1922,12 +2017,12 @@
       </c>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="18">
         <v>417</v>
@@ -1940,12 +2035,12 @@
       </c>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="18">
         <v>418</v>
@@ -1954,16 +2049,16 @@
         <v>0</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F36" s="17"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37" s="18">
         <v>419</v>
@@ -1972,16 +2067,16 @@
         <v>0</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C38" s="18">
         <v>420</v>
@@ -1990,16 +2085,16 @@
         <v>0</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C39" s="18">
         <v>421</v>
@@ -2008,16 +2103,16 @@
         <v>0</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" s="18">
         <v>422</v>
@@ -2026,16 +2121,16 @@
         <v>0</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="49" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C41" s="18">
         <v>423</v>
@@ -2044,16 +2139,16 @@
         <v>0</v>
       </c>
       <c r="E41" s="50" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C42" s="18">
         <v>424</v>
@@ -2061,15 +2156,15 @@
       <c r="D42" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E42" s="53" t="s">
-        <v>203</v>
+      <c r="E42" s="52" t="s">
+        <v>200</v>
       </c>
       <c r="F42" s="17"/>
     </row>
-    <row r="43" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="31"/>
       <c r="B43" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C43" s="29">
         <v>501</v>
@@ -2082,12 +2177,12 @@
       </c>
       <c r="F43" s="28"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C44" s="33">
         <v>502</v>
@@ -2100,12 +2195,12 @@
       </c>
       <c r="F44" s="32"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C45" s="33">
         <v>503</v>
@@ -2118,12 +2213,12 @@
       </c>
       <c r="F45" s="32"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C46" s="33">
         <v>504</v>
@@ -2136,10 +2231,10 @@
       </c>
       <c r="F46" s="32"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="31"/>
       <c r="B47" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C47" s="29">
         <v>505</v>
@@ -2152,12 +2247,12 @@
       </c>
       <c r="F47" s="28"/>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C48" s="33">
         <v>506</v>
@@ -2172,12 +2267,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C49" s="33">
         <v>507</v>
@@ -2190,12 +2285,12 @@
       </c>
       <c r="F49" s="32"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B50" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" s="33">
         <v>508</v>
@@ -2208,12 +2303,12 @@
       </c>
       <c r="F50" s="32"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B51" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C51" s="33">
         <v>509</v>
@@ -2222,16 +2317,16 @@
         <v>0</v>
       </c>
       <c r="E51" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F51" s="32"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B52" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52" s="33">
         <v>510</v>
@@ -2240,16 +2335,16 @@
         <v>0</v>
       </c>
       <c r="E52" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F52" s="32"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="35" t="s">
         <v>40</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C53" s="33">
         <v>511</v>
@@ -2262,12 +2357,12 @@
       </c>
       <c r="F53" s="32"/>
     </row>
-    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="35" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C54" s="33">
         <v>512</v>
@@ -2276,16 +2371,16 @@
         <v>0</v>
       </c>
       <c r="E54" s="35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F54" s="32"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55" s="37">
         <v>601</v>
@@ -2298,12 +2393,12 @@
       </c>
       <c r="F55" s="36"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C56" s="37">
         <v>602</v>
@@ -2316,12 +2411,12 @@
       </c>
       <c r="F56" s="36"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="39" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C57" s="37">
         <v>603</v>
@@ -2334,12 +2429,12 @@
       </c>
       <c r="F57" s="36"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C58" s="37">
         <v>604</v>
@@ -2348,16 +2443,16 @@
         <v>1</v>
       </c>
       <c r="E58" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="F58" s="36"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="F58" s="36"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="39" t="s">
-        <v>122</v>
-      </c>
       <c r="B59" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59" s="37">
         <v>605</v>
@@ -2366,16 +2461,16 @@
         <v>0</v>
       </c>
       <c r="E59" s="39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F59" s="36"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="39" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C60" s="37">
         <v>606</v>
@@ -2390,12 +2485,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="39" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C61" s="37">
         <v>607</v>
@@ -2408,12 +2503,12 @@
       </c>
       <c r="F61" s="36"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="39" t="s">
         <v>43</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C62" s="37">
         <v>608</v>
@@ -2426,12 +2521,12 @@
       </c>
       <c r="F62" s="36"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C63" s="37">
         <v>609</v>
@@ -2444,12 +2539,12 @@
       </c>
       <c r="F63" s="36"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="39" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C64" s="37">
         <v>610</v>
@@ -2458,16 +2553,16 @@
         <v>0</v>
       </c>
       <c r="E64" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F64" s="36"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="39" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C65" s="37">
         <v>611</v>
@@ -2476,16 +2571,16 @@
         <v>1</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F65" s="36"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C66" s="37">
         <v>612</v>
@@ -2500,12 +2595,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C67" s="37">
         <v>613</v>
@@ -2514,16 +2609,16 @@
         <v>0</v>
       </c>
       <c r="E67" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="F67" s="36"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="F67" s="36"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="39" t="s">
-        <v>152</v>
-      </c>
       <c r="B68" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C68" s="37">
         <v>614</v>
@@ -2532,16 +2627,16 @@
         <v>0</v>
       </c>
       <c r="E68" s="39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F68" s="36"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="39" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C69" s="37">
         <v>615</v>
@@ -2550,16 +2645,16 @@
         <v>0</v>
       </c>
       <c r="E69" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F69" s="36"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C70" s="37">
         <v>616</v>
@@ -2568,16 +2663,16 @@
         <v>0</v>
       </c>
       <c r="E70" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F70" s="36"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="39" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C71" s="37">
         <v>617</v>
@@ -2586,16 +2681,16 @@
         <v>0</v>
       </c>
       <c r="E71" s="39" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F71" s="36"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="39" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C72" s="37">
         <v>618</v>
@@ -2604,16 +2699,16 @@
         <v>0</v>
       </c>
       <c r="E72" s="39" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F72" s="36"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="52" t="s">
-        <v>201</v>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="53" t="s">
+        <v>198</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C73" s="37">
         <v>619</v>
@@ -2626,151 +2721,143 @@
       </c>
       <c r="F73" s="36"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="27" t="s">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="53" t="s">
+        <v>204</v>
+      </c>
+      <c r="B74" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C74" s="37">
+        <v>620</v>
+      </c>
+      <c r="D74" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="F74" s="36"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="55" t="s">
+        <v>206</v>
+      </c>
+      <c r="B75" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" s="37">
+        <v>621</v>
+      </c>
+      <c r="D75" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="F75" s="36"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="55" t="s">
+        <v>210</v>
+      </c>
+      <c r="B76" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76" s="37">
+        <v>622</v>
+      </c>
+      <c r="D76" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="56" t="s">
+        <v>209</v>
+      </c>
+      <c r="F76" s="36"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="55" t="s">
+        <v>211</v>
+      </c>
+      <c r="B77" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C77" s="37">
+        <v>623</v>
+      </c>
+      <c r="D77" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E77" s="57" t="s">
+        <v>165</v>
+      </c>
+      <c r="F77" s="36"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B78" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C78" s="25">
+        <v>701</v>
+      </c>
+      <c r="D78" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E78" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F78" s="24"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="B79" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C79" s="25">
+        <v>702</v>
+      </c>
+      <c r="D79" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E79" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B80" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C80" s="25">
+        <v>703</v>
+      </c>
+      <c r="D80" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E80" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F80" s="24"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="B74" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C74" s="25">
-        <v>701</v>
-      </c>
-      <c r="D74" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E74" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F74" s="24"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B75" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C75" s="25">
-        <v>702</v>
-      </c>
-      <c r="D75" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E75" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F75" s="24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="B76" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C76" s="25">
-        <v>703</v>
-      </c>
-      <c r="D76" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E76" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F76" s="24"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B77" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C77" s="25">
+      <c r="B81" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C81" s="25">
         <v>704</v>
-      </c>
-      <c r="D77" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E77" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F77" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="B78" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C78" s="25">
-        <v>705</v>
-      </c>
-      <c r="D78" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E78" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F78" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B79" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C79" s="25">
-        <v>706</v>
-      </c>
-      <c r="D79" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E79" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F79" s="24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="B80" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C80" s="25">
-        <v>707</v>
-      </c>
-      <c r="D80" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E80" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F80" s="24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B81" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C81" s="25">
-        <v>708</v>
       </c>
       <c r="D81" s="26" t="s">
         <v>0</v>
@@ -2779,18 +2866,18 @@
         <v>10</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="27" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B82" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C82" s="25">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="D82" s="26" t="s">
         <v>0</v>
@@ -2799,344 +2886,352 @@
         <v>10</v>
       </c>
       <c r="F82" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B83" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C83" s="25">
+        <v>706</v>
+      </c>
+      <c r="D83" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E83" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B84" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C84" s="25">
+        <v>707</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B85" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C85" s="25">
+        <v>708</v>
+      </c>
+      <c r="D85" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" s="24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="27" t="s">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="B86" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C86" s="25">
+        <v>709</v>
+      </c>
+      <c r="D86" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E86" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B87" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C87" s="25">
+        <v>710</v>
+      </c>
+      <c r="D87" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="F87" s="24"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B88" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C88" s="25">
+        <v>711</v>
+      </c>
+      <c r="D88" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E88" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F88" s="24"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B89" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C89" s="25">
+        <v>712</v>
+      </c>
+      <c r="D89" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E89" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F89" s="24"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="B83" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C83" s="25">
-        <v>710</v>
-      </c>
-      <c r="D83" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E83" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F83" s="24"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="27" t="s">
+      <c r="B90" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C90" s="25">
+        <v>713</v>
+      </c>
+      <c r="D90" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E90" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="F90" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="B84" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C84" s="25">
-        <v>711</v>
-      </c>
-      <c r="D84" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E84" s="27" t="s">
+      <c r="B91" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C91" s="25">
+        <v>714</v>
+      </c>
+      <c r="D91" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E91" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="F91" s="24"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B92" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C92" s="25">
+        <v>715</v>
+      </c>
+      <c r="D92" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E92" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F92" s="24"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="B93" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C93" s="25">
+        <v>716</v>
+      </c>
+      <c r="D93" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F84" s="24"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="B85" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C85" s="25">
-        <v>712</v>
-      </c>
-      <c r="D85" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E85" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="F85" s="24"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="27" t="s">
-        <v>138</v>
-      </c>
-      <c r="B86" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C86" s="25">
-        <v>713</v>
-      </c>
-      <c r="D86" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E86" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F86" s="24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="B87" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C87" s="25">
-        <v>714</v>
-      </c>
-      <c r="D87" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E87" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="F87" s="24"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="27" t="s">
+      <c r="F93" s="24"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="B94" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C94" s="25">
+        <v>717</v>
+      </c>
+      <c r="D94" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E94" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F94" s="24"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="B95" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C95" s="25">
+        <v>718</v>
+      </c>
+      <c r="D95" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E95" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="F95" s="24"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="B96" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C96" s="25">
+        <v>719</v>
+      </c>
+      <c r="D96" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E96" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="F96" s="24"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="B97" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C97" s="41">
+        <v>801</v>
+      </c>
+      <c r="D97" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E97" s="43" t="s">
+        <v>203</v>
+      </c>
+      <c r="F97" s="40"/>
+    </row>
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A98" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B98" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C98" s="41">
+        <v>802</v>
+      </c>
+      <c r="D98" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E98" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="F98" s="40"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B99" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C99" s="41">
+        <v>803</v>
+      </c>
+      <c r="D99" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F99" s="40"/>
+    </row>
+    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A100" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B100" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C100" s="41">
+        <v>804</v>
+      </c>
+      <c r="D100" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="F100" s="40"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="B88" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C88" s="25">
-        <v>715</v>
-      </c>
-      <c r="D88" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E88" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F88" s="24"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="B89" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C89" s="25">
-        <v>716</v>
-      </c>
-      <c r="D89" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E89" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F89" s="24"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="B90" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C90" s="25">
-        <v>717</v>
-      </c>
-      <c r="D90" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E90" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F90" s="24"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="27" t="s">
-        <v>183</v>
-      </c>
-      <c r="B91" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C91" s="25">
-        <v>718</v>
-      </c>
-      <c r="D91" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E91" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="F91" s="24"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="B92" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C92" s="25">
-        <v>719</v>
-      </c>
-      <c r="D92" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E92" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="F92" s="24"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="43" t="s">
-        <v>205</v>
-      </c>
-      <c r="B93" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C93" s="41">
-        <v>801</v>
-      </c>
-      <c r="D93" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E93" s="43" t="s">
-        <v>206</v>
-      </c>
-      <c r="F93" s="40"/>
-    </row>
-    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="B94" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C94" s="41">
-        <v>802</v>
-      </c>
-      <c r="D94" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E94" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="F94" s="40"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="B95" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C95" s="41">
-        <v>803</v>
-      </c>
-      <c r="D95" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E95" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="F95" s="40"/>
-    </row>
-    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B96" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C96" s="41">
-        <v>804</v>
-      </c>
-      <c r="D96" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E96" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="F96" s="40"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" s="43" t="s">
-        <v>142</v>
-      </c>
-      <c r="B97" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C97" s="41">
+      <c r="B101" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C101" s="41">
         <v>805</v>
-      </c>
-      <c r="D97" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="F97" s="40"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="B98" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C98" s="41">
-        <v>806</v>
-      </c>
-      <c r="D98" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E98" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="F98" s="40"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B99" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C99" s="41">
-        <v>807</v>
-      </c>
-      <c r="D99" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E99" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="F99" s="40"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="43" t="s">
-        <v>143</v>
-      </c>
-      <c r="B100" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C100" s="41">
-        <v>808</v>
-      </c>
-      <c r="D100" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E100" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="F100" s="40"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" s="43" t="s">
-        <v>159</v>
-      </c>
-      <c r="B101" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C101" s="41">
-        <v>809</v>
       </c>
       <c r="D101" s="42" t="s">
         <v>0</v>
@@ -3146,211 +3241,283 @@
       </c>
       <c r="F101" s="40"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="B102" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C102" s="41">
+        <v>806</v>
+      </c>
+      <c r="D102" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E102" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="F102" s="40"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B103" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C103" s="41">
+        <v>807</v>
+      </c>
+      <c r="D103" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E103" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="F103" s="40"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="B104" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C104" s="41">
+        <v>808</v>
+      </c>
+      <c r="D104" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E104" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="F104" s="40"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="B105" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C105" s="41">
+        <v>809</v>
+      </c>
+      <c r="D105" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E105" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="F105" s="40"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="B106" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C106" s="41">
+        <v>810</v>
+      </c>
+      <c r="D106" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E106" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="F106" s="40"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="B102" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C102" s="41">
-        <v>810</v>
-      </c>
-      <c r="D102" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E102" s="43" t="s">
+      <c r="B107" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C107" s="41">
+        <v>811</v>
+      </c>
+      <c r="D107" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E107" s="43" t="s">
         <v>163</v>
       </c>
-      <c r="F102" s="40"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="43" t="s">
+      <c r="F107" s="40"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="B108" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C108" s="41">
+        <v>812</v>
+      </c>
+      <c r="D108" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="B103" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C103" s="41">
-        <v>811</v>
-      </c>
-      <c r="D103" s="42" t="s">
+      <c r="F108" s="40"/>
+    </row>
+    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A109" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="B109" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C109" s="41">
+        <v>813</v>
+      </c>
+      <c r="D109" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="E103" s="43" t="s">
-        <v>166</v>
-      </c>
-      <c r="F103" s="40"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="43" t="s">
-        <v>167</v>
-      </c>
-      <c r="B104" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C104" s="41">
-        <v>812</v>
-      </c>
-      <c r="D104" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E104" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="F104" s="40"/>
-    </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="43" t="s">
-        <v>172</v>
-      </c>
-      <c r="B105" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C105" s="41">
-        <v>813</v>
-      </c>
-      <c r="D105" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="E105" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="F105" s="40"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" s="43" t="s">
-        <v>190</v>
-      </c>
-      <c r="B106" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C106" s="41">
+      <c r="E109" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="F109" s="40"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="B110" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C110" s="41">
         <v>814</v>
       </c>
-      <c r="D106" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E106" s="43" t="s">
+      <c r="D110" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E110" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="F106" s="40"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="43" t="s">
-        <v>196</v>
-      </c>
-      <c r="B107" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C107" s="41">
+      <c r="F110" s="40"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="B111" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C111" s="41">
         <v>815</v>
       </c>
-      <c r="D107" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="E107" s="43" t="s">
-        <v>197</v>
-      </c>
-      <c r="F107" s="40"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="47" t="s">
+      <c r="D111" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E111" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="F111" s="40"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B108" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C108" s="45">
+      <c r="B112" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C112" s="45">
         <v>901</v>
       </c>
-      <c r="D108" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E108" s="47" t="s">
+      <c r="D112" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E112" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="F112" s="44"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="B113" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C113" s="45">
+        <v>902</v>
+      </c>
+      <c r="D113" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E113" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="F113" s="44"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="B114" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C114" s="45">
+        <v>903</v>
+      </c>
+      <c r="D114" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E114" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F114" s="44"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="47" t="s">
         <v>145</v>
       </c>
-      <c r="F108" s="44"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="B109" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C109" s="45">
-        <v>902</v>
-      </c>
-      <c r="D109" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E109" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="F109" s="44"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="B110" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C110" s="45">
-        <v>903</v>
-      </c>
-      <c r="D110" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E110" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="F110" s="44"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="B111" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C111" s="45">
+      <c r="B115" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C115" s="45">
         <v>904</v>
       </c>
-      <c r="D111" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E111" s="47" t="s">
+      <c r="D115" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E115" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="F111" s="44"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="B112" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C112" s="45">
+      <c r="F115" s="44"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B116" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C116" s="45">
         <v>905</v>
       </c>
-      <c r="D112" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E112" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="F112" s="44"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="2"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="2"/>
-      <c r="F113" s="1"/>
+      <c r="D116" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="F116" s="44"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="2"/>
+      <c r="B117" s="2"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:E69">

</xml_diff>

<commit_message>
Cleaned up PEP8 stuff Remove whitespace from custom property names
</commit_message>
<xml_diff>
--- a/elevator_log_messages.xlsx
+++ b/elevator_log_messages.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="214">
   <si>
     <t>warn</t>
   </si>
@@ -666,6 +666,9 @@
   </si>
   <si>
     <t>Indicator %s has an observable or indicator composite expression which may not supported correctly in STIX 2.0 - please check this pattern</t>
+  </si>
+  <si>
+    <t>The custom property name %s contains whitespace, replacing it with underscores</t>
   </si>
 </sst>
 </file>
@@ -866,7 +869,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="56">
+  <cellStyleXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -899,6 +902,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1048,7 +1053,7 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="31" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="31" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="56">
+  <cellStyles count="58">
     <cellStyle name="20% - Accent2" xfId="31" builtinId="34"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1077,6 +1082,7 @@
     <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1104,6 +1110,7 @@
     <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1387,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F117"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2794,90 +2801,88 @@
       <c r="F77" s="36"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B78" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="C78" s="25">
-        <v>701</v>
-      </c>
-      <c r="D78" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E78" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F78" s="24"/>
+      <c r="A78" s="55" t="s">
+        <v>213</v>
+      </c>
+      <c r="B78" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C78" s="37">
+        <v>624</v>
+      </c>
+      <c r="D78" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="F78" s="36"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="27" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B79" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C79" s="25">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D79" s="26" t="s">
         <v>63</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F79" s="24" t="s">
-        <v>39</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F79" s="24"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="27" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B80" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C80" s="25">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D80" s="26" t="s">
         <v>63</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F80" s="24"/>
+        <v>38</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B81" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C81" s="25">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="E81" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F81" s="24" t="s">
-        <v>11</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F81" s="24"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B82" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C82" s="25">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D82" s="26" t="s">
         <v>0</v>
@@ -2891,13 +2896,13 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B83" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C83" s="25">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D83" s="26" t="s">
         <v>0</v>
@@ -2906,18 +2911,18 @@
         <v>10</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B84" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C84" s="25">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D84" s="26" t="s">
         <v>0</v>
@@ -2931,13 +2936,13 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B85" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C85" s="25">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D85" s="26" t="s">
         <v>0</v>
@@ -2946,18 +2951,18 @@
         <v>10</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B86" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C86" s="25">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D86" s="26" t="s">
         <v>0</v>
@@ -2971,553 +2976,573 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B87" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C87" s="25">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D87" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E87" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F87" s="24"/>
+        <v>10</v>
+      </c>
+      <c r="F87" s="24" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B88" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C88" s="25">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D88" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E88" s="27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F88" s="24"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="27" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
       <c r="B89" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C89" s="25">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D89" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E89" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F89" s="24"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="27" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="B90" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C90" s="25">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D90" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E90" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F90" s="24" t="s">
-        <v>35</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F90" s="24"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B91" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C91" s="25">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D91" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E91" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="F91" s="24"/>
+        <v>34</v>
+      </c>
+      <c r="F91" s="24" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B92" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C92" s="25">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D92" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E92" s="27" t="s">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="F92" s="24"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B93" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C93" s="25">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D93" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E93" s="27" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F93" s="24"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="27" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="B94" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C94" s="25">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D94" s="26" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="E94" s="27" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F94" s="24"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="27" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="B95" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C95" s="25">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D95" s="26" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="E95" s="27" t="s">
-        <v>179</v>
+        <v>29</v>
       </c>
       <c r="F95" s="24"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="27" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B96" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C96" s="25">
+        <v>718</v>
+      </c>
+      <c r="D96" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E96" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="F96" s="24"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="B97" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C97" s="25">
         <v>719</v>
       </c>
-      <c r="D96" s="26" t="s">
+      <c r="D97" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E96" s="27" t="s">
+      <c r="E97" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="F96" s="24"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="43" t="s">
+      <c r="F97" s="24"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="43" t="s">
         <v>202</v>
-      </c>
-      <c r="B97" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="C97" s="41">
-        <v>801</v>
-      </c>
-      <c r="D97" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E97" s="43" t="s">
-        <v>203</v>
-      </c>
-      <c r="F97" s="40"/>
-    </row>
-    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A98" s="43" t="s">
-        <v>42</v>
       </c>
       <c r="B98" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C98" s="41">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D98" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E98" s="43" t="s">
-        <v>56</v>
+        <v>203</v>
       </c>
       <c r="F98" s="40"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A99" s="43" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B99" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C99" s="41">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D99" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E99" s="43" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="F99" s="40"/>
     </row>
-    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B100" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C100" s="41">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D100" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E100" s="43" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="F100" s="40"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A101" s="43" t="s">
-        <v>140</v>
+        <v>47</v>
       </c>
       <c r="B101" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C101" s="41">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D101" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E101" s="43" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F101" s="40"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="43" t="s">
-        <v>208</v>
+        <v>140</v>
       </c>
       <c r="B102" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C102" s="41">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D102" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E102" s="43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F102" s="40"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="43" t="s">
-        <v>52</v>
+        <v>208</v>
       </c>
       <c r="B103" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C103" s="41">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D103" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E103" s="43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F103" s="40"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="43" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
       <c r="B104" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C104" s="41">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D104" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E104" s="43" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F104" s="40"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="43" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="B105" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C105" s="41">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D105" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E105" s="43" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F105" s="40"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="43" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B106" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C106" s="41">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D106" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E106" s="43" t="s">
-        <v>161</v>
+        <v>48</v>
       </c>
       <c r="F106" s="40"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="43" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B107" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C107" s="41">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D107" s="42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F107" s="40"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="43" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B108" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C108" s="41">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D108" s="42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E108" s="43" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F108" s="40"/>
     </row>
-    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="43" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B109" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C109" s="41">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D109" s="42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E109" s="43" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F109" s="40"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A110" s="43" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="B110" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C110" s="41">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D110" s="42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110" s="43" t="s">
-        <v>18</v>
+        <v>170</v>
       </c>
       <c r="F110" s="40"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="43" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B111" s="43" t="s">
         <v>65</v>
       </c>
       <c r="C111" s="41">
+        <v>814</v>
+      </c>
+      <c r="D111" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E111" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F111" s="40"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="B112" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C112" s="41">
         <v>815</v>
       </c>
-      <c r="D111" s="42" t="s">
+      <c r="D112" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="E111" s="43" t="s">
+      <c r="E112" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="F111" s="40"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B112" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C112" s="45">
-        <v>901</v>
-      </c>
-      <c r="D112" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="E112" s="47" t="s">
-        <v>143</v>
-      </c>
-      <c r="F112" s="44"/>
+      <c r="F112" s="40"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="47" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="B113" s="47" t="s">
         <v>70</v>
       </c>
       <c r="C113" s="45">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D113" s="46" t="s">
         <v>63</v>
       </c>
       <c r="E113" s="47" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F113" s="44"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="47" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B114" s="47" t="s">
         <v>70</v>
       </c>
       <c r="C114" s="45">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D114" s="46" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="E114" s="47" t="s">
-        <v>27</v>
+        <v>147</v>
       </c>
       <c r="F114" s="44"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B115" s="47" t="s">
         <v>70</v>
       </c>
       <c r="C115" s="45">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D115" s="46" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="E115" s="47" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F115" s="44"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="47" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B116" s="47" t="s">
         <v>70</v>
       </c>
       <c r="C116" s="45">
+        <v>904</v>
+      </c>
+      <c r="D116" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E116" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="F116" s="44"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B117" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C117" s="45">
         <v>905</v>
       </c>
-      <c r="D116" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E116" s="47" t="s">
+      <c r="D117" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E117" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="F116" s="44"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="2"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="1"/>
-      <c r="E117" s="2"/>
-      <c r="F117" s="1"/>
+      <c r="F117" s="44"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="2"/>
+      <c r="B118" s="2"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:E69">

</xml_diff>

<commit_message>
fixed json gold test cases for escaping backslash and single quote replaced CybOX with STIX in messages replaced "extended_properties" be new name "extensions" escaping backslash and single quote use IN operator for lists on rhs, if the operator is = only call text_type in to_string
</commit_message>
<xml_diff>
--- a/elevator_log_messages.xlsx
+++ b/elevator_log_messages.xlsx
@@ -191,12 +191,6 @@
     <t>convert_windows_executable_file_to_pattern</t>
   </si>
   <si>
-    <t>The exports property of WinExecutableFileObj is not part of Cybox 3.0</t>
-  </si>
-  <si>
-    <t>The imports property of WinExecutableFileObj is not part of Cybox 3.0</t>
-  </si>
-  <si>
     <t>convert_file/convert_file_name_and_path_to_pattern</t>
   </si>
   <si>
@@ -494,18 +488,12 @@
     <t>convert_process_to_pattern</t>
   </si>
   <si>
-    <t>Windows Handles are not a part of CybOX 3.0</t>
-  </si>
-  <si>
     <t>Threat actor [id] title is used for name property</t>
   </si>
   <si>
     <t>Related Objects of cyber observables for [id] are not handled yet</t>
   </si>
   <si>
-    <t>The address type [address] is not part of Cybox 3.0</t>
-  </si>
-  <si>
     <t>convert_address</t>
   </si>
   <si>
@@ -669,6 +657,18 @@
   </si>
   <si>
     <t>The custom property name %s contains whitespace, replacing it with underscores</t>
+  </si>
+  <si>
+    <t>The exports property of WinExecutableFileObj is not part of STIX 2.0</t>
+  </si>
+  <si>
+    <t>The imports property of WinExecutableFileObj is not part of STIX 2.0</t>
+  </si>
+  <si>
+    <t>Windows Handles are not a part of STIX 2.0</t>
+  </si>
+  <si>
+    <t>The address type [address] is not part of STIX 2.0</t>
   </si>
 </sst>
 </file>
@@ -1396,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1415,13 +1415,13 @@
         <v>2</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>3</v>
@@ -1440,10 +1440,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3" s="11">
         <v>201</v>
@@ -1452,18 +1452,18 @@
         <v>0</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" s="11">
         <v>202</v>
@@ -1472,16 +1472,16 @@
         <v>1</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="11">
         <v>203</v>
@@ -1490,34 +1490,34 @@
         <v>1</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="11">
         <v>204</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="11">
         <v>205</v>
@@ -1532,10 +1532,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" s="11">
         <v>206</v>
@@ -1550,10 +1550,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C9" s="11">
         <v>207</v>
@@ -1562,16 +1562,16 @@
         <v>1</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F9" s="10"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="11">
         <v>208</v>
@@ -1583,15 +1583,15 @@
         <v>38</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C11" s="11">
         <v>209</v>
@@ -1600,16 +1600,16 @@
         <v>0</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C12" s="11">
         <v>210</v>
@@ -1618,16 +1618,16 @@
         <v>1</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="15">
         <v>301</v>
@@ -1644,10 +1644,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" s="15">
         <v>302</v>
@@ -1662,16 +1662,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C15" s="15">
         <v>303</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>19</v>
@@ -1680,10 +1680,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C16" s="15">
         <v>304</v>
@@ -1692,16 +1692,16 @@
         <v>0</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C17" s="15">
         <v>305</v>
@@ -1710,16 +1710,16 @@
         <v>0</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C18" s="15">
         <v>306</v>
@@ -1728,16 +1728,16 @@
         <v>0</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" s="18">
         <v>401</v>
@@ -1752,10 +1752,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="18">
         <v>402</v>
@@ -1764,16 +1764,16 @@
         <v>0</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="18">
         <v>403</v>
@@ -1790,10 +1790,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" s="18">
         <v>404</v>
@@ -1810,10 +1810,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C23" s="18">
         <v>405</v>
@@ -1828,10 +1828,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="18">
         <v>406</v>
@@ -1846,10 +1846,10 @@
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" s="18">
         <v>407</v>
@@ -1864,10 +1864,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="18">
         <v>408</v>
@@ -1882,10 +1882,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" s="18">
         <v>409</v>
@@ -1900,10 +1900,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C28" s="18">
         <v>410</v>
@@ -1918,10 +1918,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C29" s="18">
         <v>411</v>
@@ -1936,10 +1936,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30" s="18">
         <v>412</v>
@@ -1954,10 +1954,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C31" s="18">
         <v>413</v>
@@ -1972,10 +1972,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C32" s="18">
         <v>414</v>
@@ -1990,10 +1990,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C33" s="18">
         <v>415</v>
@@ -2008,10 +2008,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C34" s="18">
         <v>416</v>
@@ -2026,10 +2026,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C35" s="18">
         <v>417</v>
@@ -2044,10 +2044,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
-        <v>54</v>
+        <v>210</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C36" s="18">
         <v>418</v>
@@ -2062,10 +2062,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
-        <v>55</v>
+        <v>211</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C37" s="18">
         <v>419</v>
@@ -2080,10 +2080,10 @@
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C38" s="18">
         <v>420</v>
@@ -2092,16 +2092,16 @@
         <v>0</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F38" s="17"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>158</v>
+        <v>213</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C39" s="18">
         <v>421</v>
@@ -2110,16 +2110,16 @@
         <v>0</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F39" s="17"/>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C40" s="18">
         <v>422</v>
@@ -2128,16 +2128,16 @@
         <v>0</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F40" s="17"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="49" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C41" s="18">
         <v>423</v>
@@ -2146,16 +2146,16 @@
         <v>0</v>
       </c>
       <c r="E41" s="50" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F41" s="17"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C42" s="18">
         <v>424</v>
@@ -2164,14 +2164,14 @@
         <v>0</v>
       </c>
       <c r="E42" s="52" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F42" s="17"/>
     </row>
     <row r="43" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="31"/>
       <c r="B43" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C43" s="29">
         <v>501</v>
@@ -2186,10 +2186,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="35" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C44" s="33">
         <v>502</v>
@@ -2204,10 +2204,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C45" s="33">
         <v>503</v>
@@ -2222,10 +2222,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C46" s="33">
         <v>504</v>
@@ -2241,7 +2241,7 @@
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="31"/>
       <c r="B47" s="31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C47" s="29">
         <v>505</v>
@@ -2256,10 +2256,10 @@
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C48" s="33">
         <v>506</v>
@@ -2276,10 +2276,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C49" s="33">
         <v>507</v>
@@ -2294,10 +2294,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B50" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C50" s="33">
         <v>508</v>
@@ -2312,10 +2312,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B51" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C51" s="33">
         <v>509</v>
@@ -2324,16 +2324,16 @@
         <v>0</v>
       </c>
       <c r="E51" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F51" s="32"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B52" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C52" s="33">
         <v>510</v>
@@ -2342,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F52" s="32"/>
     </row>
@@ -2351,7 +2351,7 @@
         <v>40</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C53" s="33">
         <v>511</v>
@@ -2366,10 +2366,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="35" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B54" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C54" s="33">
         <v>512</v>
@@ -2378,16 +2378,16 @@
         <v>0</v>
       </c>
       <c r="E54" s="35" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F54" s="32"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="39" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B55" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C55" s="37">
         <v>601</v>
@@ -2402,10 +2402,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="39" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B56" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C56" s="37">
         <v>602</v>
@@ -2420,10 +2420,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="39" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B57" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C57" s="37">
         <v>603</v>
@@ -2438,10 +2438,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C58" s="37">
         <v>604</v>
@@ -2450,16 +2450,16 @@
         <v>1</v>
       </c>
       <c r="E58" s="39" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F58" s="36"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="39" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B59" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C59" s="37">
         <v>605</v>
@@ -2468,16 +2468,16 @@
         <v>0</v>
       </c>
       <c r="E59" s="39" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F59" s="36"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B60" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C60" s="37">
         <v>606</v>
@@ -2494,10 +2494,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="39" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B61" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C61" s="37">
         <v>607</v>
@@ -2515,7 +2515,7 @@
         <v>43</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C62" s="37">
         <v>608</v>
@@ -2530,10 +2530,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="39" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B63" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C63" s="37">
         <v>609</v>
@@ -2548,10 +2548,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="39" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B64" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C64" s="37">
         <v>610</v>
@@ -2560,16 +2560,16 @@
         <v>0</v>
       </c>
       <c r="E64" s="39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F64" s="36"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="39" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B65" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C65" s="37">
         <v>611</v>
@@ -2578,16 +2578,16 @@
         <v>1</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F65" s="36"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="39" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B66" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C66" s="37">
         <v>612</v>
@@ -2604,10 +2604,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C67" s="37">
         <v>613</v>
@@ -2616,16 +2616,16 @@
         <v>0</v>
       </c>
       <c r="E67" s="39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F67" s="36"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B68" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C68" s="37">
         <v>614</v>
@@ -2634,16 +2634,16 @@
         <v>0</v>
       </c>
       <c r="E68" s="39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F68" s="36"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B69" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C69" s="37">
         <v>615</v>
@@ -2652,16 +2652,16 @@
         <v>0</v>
       </c>
       <c r="E69" s="39" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F69" s="36"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="39" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B70" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C70" s="37">
         <v>616</v>
@@ -2670,16 +2670,16 @@
         <v>0</v>
       </c>
       <c r="E70" s="39" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F70" s="36"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="39" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B71" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C71" s="37">
         <v>617</v>
@@ -2688,16 +2688,16 @@
         <v>0</v>
       </c>
       <c r="E71" s="39" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F71" s="36"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="39" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B72" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C72" s="37">
         <v>618</v>
@@ -2706,16 +2706,16 @@
         <v>0</v>
       </c>
       <c r="E72" s="39" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F72" s="36"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="53" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B73" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C73" s="37">
         <v>619</v>
@@ -2730,10 +2730,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="53" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B74" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C74" s="37">
         <v>620</v>
@@ -2742,16 +2742,16 @@
         <v>0</v>
       </c>
       <c r="E74" s="54" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F74" s="36"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="55" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B75" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C75" s="37">
         <v>621</v>
@@ -2766,10 +2766,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="55" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B76" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C76" s="37">
         <v>622</v>
@@ -2778,16 +2778,16 @@
         <v>0</v>
       </c>
       <c r="E76" s="56" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F76" s="36"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="55" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B77" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C77" s="37">
         <v>623</v>
@@ -2796,16 +2796,16 @@
         <v>0</v>
       </c>
       <c r="E77" s="57" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F77" s="36"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="55" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B78" s="39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C78" s="37">
         <v>624</v>
@@ -2814,22 +2814,22 @@
         <v>0</v>
       </c>
       <c r="E78" s="55" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F78" s="36"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="27" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B79" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C79" s="25">
         <v>701</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E79" s="27" t="s">
         <v>29</v>
@@ -2838,16 +2838,16 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B80" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C80" s="25">
         <v>702</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E80" s="27" t="s">
         <v>38</v>
@@ -2858,28 +2858,28 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C81" s="25">
         <v>703</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E81" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F81" s="24"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B82" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C82" s="25">
         <v>704</v>
@@ -2896,10 +2896,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B83" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C83" s="25">
         <v>705</v>
@@ -2916,10 +2916,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C84" s="25">
         <v>706</v>
@@ -2936,10 +2936,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C85" s="25">
         <v>707</v>
@@ -2956,10 +2956,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B86" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C86" s="25">
         <v>708</v>
@@ -2976,10 +2976,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B87" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C87" s="25">
         <v>709</v>
@@ -2996,10 +2996,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B88" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C88" s="25">
         <v>710</v>
@@ -3014,10 +3014,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B89" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C89" s="25">
         <v>711</v>
@@ -3032,10 +3032,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B90" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C90" s="25">
         <v>712</v>
@@ -3050,10 +3050,10 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B91" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C91" s="25">
         <v>713</v>
@@ -3070,10 +3070,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B92" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C92" s="25">
         <v>714</v>
@@ -3082,16 +3082,16 @@
         <v>0</v>
       </c>
       <c r="E92" s="27" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F92" s="24"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="27" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B93" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C93" s="25">
         <v>715</v>
@@ -3106,10 +3106,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="27" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B94" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C94" s="25">
         <v>716</v>
@@ -3124,16 +3124,16 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="27" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B95" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C95" s="25">
         <v>717</v>
       </c>
       <c r="D95" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E95" s="27" t="s">
         <v>29</v>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="27" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B96" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C96" s="25">
         <v>718</v>
@@ -3154,34 +3154,34 @@
         <v>0</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F96" s="24"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="27" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B97" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C97" s="25">
         <v>719</v>
       </c>
       <c r="D97" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E97" s="27" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F97" s="24"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="43" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B98" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C98" s="41">
         <v>801</v>
@@ -3190,7 +3190,7 @@
         <v>0</v>
       </c>
       <c r="E98" s="43" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F98" s="40"/>
     </row>
@@ -3199,7 +3199,7 @@
         <v>42</v>
       </c>
       <c r="B99" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C99" s="41">
         <v>802</v>
@@ -3208,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="E99" s="43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F99" s="40"/>
     </row>
@@ -3217,7 +3217,7 @@
         <v>45</v>
       </c>
       <c r="B100" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C100" s="41">
         <v>803</v>
@@ -3235,7 +3235,7 @@
         <v>47</v>
       </c>
       <c r="B101" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C101" s="41">
         <v>804</v>
@@ -3244,16 +3244,16 @@
         <v>0</v>
       </c>
       <c r="E101" s="43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F101" s="40"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B102" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C102" s="41">
         <v>805</v>
@@ -3268,10 +3268,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="43" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B103" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C103" s="41">
         <v>806</v>
@@ -3289,7 +3289,7 @@
         <v>52</v>
       </c>
       <c r="B104" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C104" s="41">
         <v>807</v>
@@ -3304,10 +3304,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="43" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B105" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C105" s="41">
         <v>808</v>
@@ -3316,16 +3316,16 @@
         <v>0</v>
       </c>
       <c r="E105" s="43" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F105" s="40"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="43" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B106" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C106" s="41">
         <v>809</v>
@@ -3340,10 +3340,10 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="43" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B107" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C107" s="41">
         <v>810</v>
@@ -3352,16 +3352,16 @@
         <v>0</v>
       </c>
       <c r="E107" s="43" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F107" s="40"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="43" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B108" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C108" s="41">
         <v>811</v>
@@ -3370,16 +3370,16 @@
         <v>1</v>
       </c>
       <c r="E108" s="43" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F108" s="40"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="43" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B109" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C109" s="41">
         <v>812</v>
@@ -3388,16 +3388,16 @@
         <v>0</v>
       </c>
       <c r="E109" s="43" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F109" s="40"/>
     </row>
     <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A110" s="43" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B110" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C110" s="41">
         <v>813</v>
@@ -3406,16 +3406,16 @@
         <v>1</v>
       </c>
       <c r="E110" s="43" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F110" s="40"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="43" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B111" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C111" s="41">
         <v>814</v>
@@ -3430,19 +3430,19 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="43" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B112" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C112" s="41">
         <v>815</v>
       </c>
       <c r="D112" s="42" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E112" s="43" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F112" s="40"/>
     </row>
@@ -3451,43 +3451,43 @@
         <v>28</v>
       </c>
       <c r="B113" s="47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C113" s="45">
         <v>901</v>
       </c>
       <c r="D113" s="46" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E113" s="47" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F113" s="44"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="47" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B114" s="47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C114" s="45">
         <v>902</v>
       </c>
       <c r="D114" s="46" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E114" s="47" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F114" s="44"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="47" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B115" s="47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C115" s="45">
         <v>903</v>
@@ -3502,16 +3502,16 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="47" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B116" s="47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C116" s="45">
         <v>904</v>
       </c>
       <c r="D116" s="46" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E116" s="47" t="s">
         <v>32</v>
@@ -3520,10 +3520,10 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="47" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B117" s="47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C117" s="45">
         <v>905</v>
@@ -3532,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="E117" s="47" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F117" s="44"/>
     </row>

</xml_diff>

<commit_message>
Applied stixmarx, data markings support, changes to logger, changes to get_identity_from_package().
</commit_message>
<xml_diff>
--- a/elevator_log_messages.xlsx
+++ b/elevator_log_messages.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="211">
   <si>
     <t>warn</t>
   </si>
@@ -648,6 +648,18 @@
   </si>
   <si>
     <t>convert_marking_specification</t>
+  </si>
+  <si>
+    <t>Found duplicate marking structure [id]</t>
+  </si>
+  <si>
+    <t>Occurs when Markings hash to the same value (internally there equal)</t>
+  </si>
+  <si>
+    <t>If Marking look_up() fails, the marking details cannot be extracted.</t>
+  </si>
+  <si>
+    <t>convert_controlled_vocabs_to_open_vocabs, get_identity_from_package</t>
   </si>
 </sst>
 </file>
@@ -855,7 +867,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -974,6 +986,8 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="31" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="31"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="31" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="31" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="20% - Accent2" xfId="31" builtinId="34"/>
@@ -1292,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E93" sqref="E93"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2066,49 +2080,51 @@
       </c>
       <c r="F42" s="17"/>
     </row>
-    <row r="43" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
-      <c r="B43" s="31" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="18">
+        <v>425</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
+      <c r="B44" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="29">
+      <c r="C44" s="29">
         <v>501</v>
       </c>
-      <c r="D43" s="30" t="s">
+      <c r="D44" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E43" s="31" t="s">
+      <c r="E44" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="F43" s="28"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C44" s="33">
-        <v>502</v>
-      </c>
-      <c r="D44" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F44" s="32"/>
+      <c r="F44" s="28"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="35" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C45" s="33">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D45" s="34" t="s">
         <v>0</v>
@@ -2120,121 +2136,121 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B46" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C46" s="33">
+        <v>503</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="32"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B47" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="33">
         <v>504</v>
       </c>
-      <c r="D46" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E46" s="35" t="s">
+      <c r="D47" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="F46" s="32"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="31"/>
-      <c r="B47" s="31" t="s">
+      <c r="F47" s="32"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="31"/>
+      <c r="B48" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="29">
+      <c r="C48" s="29">
         <v>505</v>
       </c>
-      <c r="D47" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E47" s="31" t="s">
+      <c r="D48" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F47" s="28"/>
-    </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="35" t="s">
+      <c r="F48" s="28"/>
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="35" t="s">
         <v>111</v>
-      </c>
-      <c r="B48" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C48" s="33">
-        <v>506</v>
-      </c>
-      <c r="D48" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="F48" s="32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="35" t="s">
-        <v>112</v>
       </c>
       <c r="B49" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C49" s="33">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D49" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E49" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="F49" s="32"/>
+        <v>25</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B50" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C50" s="33">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D50" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E50" s="35" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F50" s="32"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B51" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C51" s="33">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D51" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E51" s="35" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="F51" s="32"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B52" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C52" s="33">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D52" s="34" t="s">
         <v>0</v>
@@ -2244,69 +2260,69 @@
       </c>
       <c r="F52" s="32"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="35" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="B53" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C53" s="33">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53" s="35" t="s">
-        <v>41</v>
+        <v>210</v>
       </c>
       <c r="F53" s="32"/>
     </row>
-    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="35" t="s">
-        <v>204</v>
+        <v>40</v>
       </c>
       <c r="B54" s="35" t="s">
         <v>70</v>
       </c>
       <c r="C54" s="33">
+        <v>511</v>
+      </c>
+      <c r="D54" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F54" s="32"/>
+    </row>
+    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="B55" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="33">
         <v>512</v>
       </c>
-      <c r="D54" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E54" s="35" t="s">
+      <c r="D55" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="F54" s="32"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="39" t="s">
-        <v>116</v>
-      </c>
-      <c r="B55" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="C55" s="37">
-        <v>601</v>
-      </c>
-      <c r="D55" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="36"/>
+      <c r="F55" s="32"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B56" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C56" s="37">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D56" s="38" t="s">
         <v>0</v>
@@ -2318,52 +2334,52 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B57" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C57" s="37">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D57" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E57" s="39" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="F57" s="36"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="39" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B58" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C58" s="37">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58" s="39" t="s">
-        <v>120</v>
+        <v>38</v>
       </c>
       <c r="F58" s="36"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B59" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C59" s="37">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59" s="39" t="s">
         <v>120</v>
@@ -2372,161 +2388,161 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="39" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="B60" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C60" s="37">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D60" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="F60" s="36" t="s">
-        <v>22</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="F60" s="36"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="39" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B61" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C61" s="37">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D61" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="F61" s="36"/>
+        <v>21</v>
+      </c>
+      <c r="F61" s="36" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="39" t="s">
-        <v>43</v>
+        <v>123</v>
       </c>
       <c r="B62" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C62" s="37">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D62" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E62" s="39" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F62" s="36"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="39" t="s">
-        <v>124</v>
+        <v>43</v>
       </c>
       <c r="B63" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C63" s="37">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D63" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E63" s="39" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F63" s="36"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B64" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C64" s="37">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" s="39" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F64" s="36"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B65" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C65" s="37">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D65" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F65" s="36"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B66" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C66" s="37">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D66" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E66" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="F66" s="36" t="s">
-        <v>24</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F66" s="36"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="39" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="B67" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C67" s="37">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D67" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="F67" s="36"/>
+        <v>23</v>
+      </c>
+      <c r="F67" s="36" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B68" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C68" s="37">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D68" s="38" t="s">
         <v>0</v>
@@ -2538,31 +2554,31 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="39" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B69" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C69" s="37">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D69" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E69" s="39" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F69" s="36"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B70" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C70" s="37">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D70" s="38" t="s">
         <v>0</v>
@@ -2574,163 +2590,161 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="39" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="B71" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C71" s="37">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D71" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E71" s="39" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="F71" s="36"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="39" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B72" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C72" s="37">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D72" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E72" s="39" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F72" s="36"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="52" t="s">
-        <v>201</v>
+      <c r="A73" s="39" t="s">
+        <v>180</v>
       </c>
       <c r="B73" s="39" t="s">
         <v>73</v>
       </c>
       <c r="C73" s="37">
+        <v>618</v>
+      </c>
+      <c r="D73" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E73" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="F73" s="36"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="52" t="s">
+        <v>201</v>
+      </c>
+      <c r="B74" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C74" s="37">
         <v>619</v>
       </c>
-      <c r="D73" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E73" s="51" t="s">
+      <c r="D74" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E74" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="F73" s="36"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="B74" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C74" s="25">
-        <v>701</v>
-      </c>
-      <c r="D74" s="26" t="s">
+      <c r="F74" s="36"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="54" t="s">
+        <v>207</v>
+      </c>
+      <c r="B75" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C75" s="37">
+        <v>620</v>
+      </c>
+      <c r="D75" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E74" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F74" s="24"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B75" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C75" s="25">
-        <v>702</v>
-      </c>
-      <c r="D75" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E75" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F75" s="24" t="s">
-        <v>39</v>
+      <c r="E75" s="55" t="s">
+        <v>206</v>
+      </c>
+      <c r="F75" s="36" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B76" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C76" s="25">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D76" s="26" t="s">
         <v>64</v>
       </c>
       <c r="E76" s="27" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="F76" s="24"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="27" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B77" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C77" s="25">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D77" s="26" t="s">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="27" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B78" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C78" s="25">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E78" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F78" s="24" t="s">
-        <v>11</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F78" s="24"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B79" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C79" s="25">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="D79" s="26" t="s">
         <v>0</v>
@@ -2739,18 +2753,18 @@
         <v>10</v>
       </c>
       <c r="F79" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B80" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C80" s="25">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="D80" s="26" t="s">
         <v>0</v>
@@ -2759,18 +2773,18 @@
         <v>10</v>
       </c>
       <c r="F80" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B81" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C81" s="25">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D81" s="26" t="s">
         <v>0</v>
@@ -2779,18 +2793,18 @@
         <v>10</v>
       </c>
       <c r="F81" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B82" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C82" s="25">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="D82" s="26" t="s">
         <v>0</v>
@@ -2799,558 +2813,598 @@
         <v>10</v>
       </c>
       <c r="F82" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="27" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B83" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C83" s="25">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D83" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F83" s="24"/>
+        <v>10</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B84" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C84" s="25">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="D84" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E84" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="F84" s="24"/>
+        <v>10</v>
+      </c>
+      <c r="F84" s="24" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="27" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="B85" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C85" s="25">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D85" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F85" s="24"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B86" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C86" s="25">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D86" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E86" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F86" s="24" t="s">
-        <v>35</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F86" s="24"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="27" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
       <c r="B87" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C87" s="25">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="D87" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E87" s="27" t="s">
-        <v>171</v>
+        <v>25</v>
       </c>
       <c r="F87" s="24"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B88" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C88" s="25">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="D88" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E88" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F88" s="24"/>
+        <v>34</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B89" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C89" s="25">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D89" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E89" s="27" t="s">
-        <v>23</v>
+        <v>171</v>
       </c>
       <c r="F89" s="24"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="27" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="B90" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C90" s="25">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="D90" s="26" t="s">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E90" s="27" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="F90" s="24"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="27" t="s">
-        <v>183</v>
+        <v>141</v>
       </c>
       <c r="B91" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C91" s="25">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="D91" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E91" s="27" t="s">
-        <v>182</v>
+        <v>23</v>
       </c>
       <c r="F91" s="24"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="27" t="s">
-        <v>191</v>
+        <v>158</v>
       </c>
       <c r="B92" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C92" s="25">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D92" s="26" t="s">
         <v>64</v>
       </c>
       <c r="E92" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F92" s="24"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="B93" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C93" s="25">
+        <v>718</v>
+      </c>
+      <c r="D93" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E93" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="F93" s="24"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="B94" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C94" s="25">
+        <v>719</v>
+      </c>
+      <c r="D94" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E94" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="F92" s="24"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="43" t="s">
-        <v>205</v>
-      </c>
-      <c r="B93" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C93" s="41">
-        <v>801</v>
-      </c>
-      <c r="D93" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E93" s="43" t="s">
-        <v>206</v>
-      </c>
-      <c r="F93" s="40"/>
-    </row>
-    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="B94" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C94" s="41">
-        <v>802</v>
-      </c>
-      <c r="D94" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E94" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="F94" s="40"/>
+      <c r="F94" s="24"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="43" t="s">
-        <v>45</v>
+        <v>205</v>
       </c>
       <c r="B95" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C95" s="41">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D95" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E95" s="43" t="s">
-        <v>46</v>
+        <v>206</v>
       </c>
       <c r="F95" s="40"/>
     </row>
     <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="43" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B96" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C96" s="41">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D96" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E96" s="43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F96" s="40"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="43" t="s">
-        <v>142</v>
+        <v>45</v>
       </c>
       <c r="B97" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C97" s="41">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D97" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E97" s="43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F97" s="40"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="43" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B98" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C98" s="41">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D98" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E98" s="43" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F98" s="40"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="43" t="s">
-        <v>53</v>
+        <v>142</v>
       </c>
       <c r="B99" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C99" s="41">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="D99" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E99" s="43" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F99" s="40"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="43" t="s">
-        <v>143</v>
+        <v>51</v>
       </c>
       <c r="B100" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C100" s="41">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D100" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E100" s="43" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F100" s="40"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="43" t="s">
-        <v>159</v>
+        <v>53</v>
       </c>
       <c r="B101" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C101" s="41">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="D101" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E101" s="43" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F101" s="40"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="43" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="B102" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C102" s="41">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D102" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E102" s="43" t="s">
-        <v>163</v>
+        <v>59</v>
       </c>
       <c r="F102" s="40"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="43" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B103" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C103" s="41">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="D103" s="42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103" s="43" t="s">
-        <v>166</v>
+        <v>48</v>
       </c>
       <c r="F103" s="40"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="43" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B104" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C104" s="41">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D104" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E104" s="43" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F104" s="40"/>
     </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="43" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="B105" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C105" s="41">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="D105" s="42" t="s">
         <v>1</v>
       </c>
       <c r="E105" s="43" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="F105" s="40"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="43" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
       <c r="B106" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C106" s="41">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D106" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E106" s="43" t="s">
-        <v>18</v>
+        <v>168</v>
       </c>
       <c r="F106" s="40"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="43" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="B107" s="43" t="s">
         <v>66</v>
       </c>
       <c r="C107" s="41">
+        <v>813</v>
+      </c>
+      <c r="D107" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E107" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="F107" s="40"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="B108" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C108" s="41">
+        <v>814</v>
+      </c>
+      <c r="D108" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E108" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F108" s="40"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="B109" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C109" s="41">
         <v>815</v>
       </c>
-      <c r="D107" s="42" t="s">
+      <c r="D109" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="E107" s="43" t="s">
+      <c r="E109" s="43" t="s">
         <v>197</v>
       </c>
-      <c r="F107" s="40"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B108" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C108" s="45">
-        <v>901</v>
-      </c>
-      <c r="D108" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E108" s="47" t="s">
-        <v>145</v>
-      </c>
-      <c r="F108" s="44"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="47" t="s">
-        <v>148</v>
-      </c>
-      <c r="B109" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C109" s="45">
-        <v>902</v>
-      </c>
-      <c r="D109" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E109" s="47" t="s">
-        <v>149</v>
-      </c>
-      <c r="F109" s="44"/>
+      <c r="F109" s="40"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="47" t="s">
-        <v>146</v>
+        <v>28</v>
       </c>
       <c r="B110" s="47" t="s">
         <v>71</v>
       </c>
       <c r="C110" s="45">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="D110" s="46" t="s">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="E110" s="47" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="F110" s="44"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="47" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B111" s="47" t="s">
         <v>71</v>
       </c>
       <c r="C111" s="45">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="D111" s="46" t="s">
         <v>64</v>
       </c>
       <c r="E111" s="47" t="s">
-        <v>32</v>
+        <v>149</v>
       </c>
       <c r="F111" s="44"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="47" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B112" s="47" t="s">
         <v>71</v>
       </c>
       <c r="C112" s="45">
+        <v>903</v>
+      </c>
+      <c r="D112" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E112" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F112" s="44"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="B113" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C113" s="45">
+        <v>904</v>
+      </c>
+      <c r="D113" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E113" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="F113" s="44"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="B114" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C114" s="45">
         <v>905</v>
       </c>
-      <c r="D112" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E112" s="47" t="s">
+      <c r="D114" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E114" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="F112" s="44"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="2"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="2"/>
-      <c r="F113" s="1"/>
+      <c r="F114" s="44"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:E69">

</xml_diff>

<commit_message>
added 211 to messages
</commit_message>
<xml_diff>
--- a/elevator_log_messages.xlsx
+++ b/elevator_log_messages.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmanuelle\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rpiazza/git/cti-stix-elevator/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11355" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22820" windowHeight="17160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Error Codes - STIX Elevator" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="219">
   <si>
     <t>warn</t>
   </si>
@@ -681,12 +681,15 @@
   </si>
   <si>
     <t>If Marking look_up() fails, the marking details cannot be extracted.</t>
+  </si>
+  <si>
+    <t>silent option is not compatible with a policy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1412,23 +1415,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="77.125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="77.1640625" style="23" customWidth="1"/>
     <col min="2" max="2" width="49" style="23" customWidth="1"/>
-    <col min="3" max="3" width="7.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="7.625" customWidth="1"/>
-    <col min="5" max="5" width="40.125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" style="23" customWidth="1"/>
     <col min="6" max="6" width="65.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="9"/>
@@ -1456,7 +1459,7 @@
       <c r="E2" s="20"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>76</v>
       </c>
@@ -1476,7 +1479,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>167</v>
       </c>
@@ -1494,7 +1497,7 @@
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
         <v>188</v>
       </c>
@@ -1512,7 +1515,7 @@
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
         <v>170</v>
       </c>
@@ -1530,7 +1533,7 @@
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
         <v>177</v>
       </c>
@@ -1548,7 +1551,7 @@
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
         <v>178</v>
       </c>
@@ -1566,7 +1569,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
         <v>179</v>
       </c>
@@ -1584,7 +1587,7 @@
       </c>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
         <v>186</v>
       </c>
@@ -1604,7 +1607,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
         <v>191</v>
       </c>
@@ -1622,7 +1625,7 @@
       </c>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>193</v>
       </c>
@@ -1640,219 +1643,219 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="11">
+        <v>211</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
         <v>79</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="15">
-        <v>301</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C14" s="15">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C15" s="15">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F15" s="14"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C16" s="15">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C17" s="15">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" s="14"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>66</v>
       </c>
       <c r="C18" s="15">
+        <v>305</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="15">
         <v>306</v>
       </c>
-      <c r="D18" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="13" t="s">
+      <c r="D19" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
         <v>85</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="18">
-        <v>401</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>86</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C20" s="18">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
       <c r="F20" s="17"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C21" s="18">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C22" s="18">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B23" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C23" s="18">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="17"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C24" s="18">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>0</v>
@@ -1862,87 +1865,87 @@
       </c>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
-        <v>208</v>
+        <v>90</v>
       </c>
       <c r="B25" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C25" s="18">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F25" s="17"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
-        <v>91</v>
+        <v>208</v>
       </c>
       <c r="B26" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C26" s="18">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B27" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C27" s="18">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F27" s="17"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C28" s="18">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B29" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C29" s="18">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>0</v>
@@ -1952,15 +1955,15 @@
       </c>
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C30" s="18">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>0</v>
@@ -1970,33 +1973,33 @@
       </c>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B31" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C31" s="18">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B32" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C32" s="18">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>0</v>
@@ -2006,15 +2009,15 @@
       </c>
       <c r="F32" s="17"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B33" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C33" s="18">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>0</v>
@@ -2024,69 +2027,69 @@
       </c>
       <c r="F33" s="17"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C34" s="18">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F34" s="17"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B35" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C35" s="18">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F35" s="17"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
-        <v>210</v>
+        <v>100</v>
       </c>
       <c r="B36" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C36" s="18">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F36" s="17"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B37" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C37" s="18">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D37" s="19" t="s">
         <v>0</v>
@@ -2096,159 +2099,159 @@
       </c>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B38" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C38" s="18">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D38" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>149</v>
+        <v>53</v>
       </c>
       <c r="F38" s="17"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B39" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C39" s="18">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D39" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F39" s="17"/>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B40" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C40" s="18">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D40" s="19" t="s">
         <v>0</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="49" t="s">
-        <v>181</v>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A41" s="22" t="s">
+        <v>203</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C41" s="18">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D41" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E41" s="50" t="s">
-        <v>182</v>
+      <c r="E41" s="22" t="s">
+        <v>172</v>
       </c>
       <c r="F41" s="17"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
-        <v>195</v>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="49" t="s">
+        <v>181</v>
       </c>
       <c r="B42" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C42" s="18">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E42" s="52" t="s">
-        <v>196</v>
+      <c r="E42" s="50" t="s">
+        <v>182</v>
       </c>
       <c r="F42" s="17"/>
     </row>
-    <row r="43" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B43" s="22" t="s">
         <v>65</v>
       </c>
       <c r="C43" s="18">
+        <v>424</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="52" t="s">
+        <v>196</v>
+      </c>
+      <c r="F43" s="17"/>
+    </row>
+    <row r="44" spans="1:6" s="48" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="18">
         <v>425</v>
       </c>
-      <c r="D43" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" s="52" t="s">
+      <c r="D44" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="F43" s="17" t="s">
+      <c r="F44" s="17" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="31" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="31"/>
+      <c r="B45" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="29">
+      <c r="C45" s="29">
         <v>501</v>
       </c>
-      <c r="D44" s="30" t="s">
+      <c r="D45" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E44" s="31" t="s">
+      <c r="E45" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="F44" s="28"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="35" t="s">
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="35" t="s">
         <v>102</v>
-      </c>
-      <c r="B45" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C45" s="33">
-        <v>502</v>
-      </c>
-      <c r="D45" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="32"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
-        <v>104</v>
       </c>
       <c r="B46" s="35" t="s">
         <v>67</v>
       </c>
       <c r="C46" s="33">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D46" s="34" t="s">
         <v>0</v>
@@ -2258,123 +2261,123 @@
       </c>
       <c r="F46" s="32"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B47" s="35" t="s">
         <v>67</v>
       </c>
       <c r="C47" s="33">
+        <v>503</v>
+      </c>
+      <c r="D47" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47" s="32"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="33">
         <v>504</v>
       </c>
-      <c r="D47" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E47" s="35" t="s">
+      <c r="D48" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="F47" s="32"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31" t="s">
+      <c r="F48" s="32"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="31"/>
+      <c r="B49" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C48" s="29">
+      <c r="C49" s="29">
         <v>505</v>
       </c>
-      <c r="D48" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="31" t="s">
+      <c r="D49" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="F48" s="28"/>
-    </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="35" t="s">
+      <c r="F49" s="28"/>
+    </row>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A50" s="35" t="s">
         <v>107</v>
-      </c>
-      <c r="B49" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" s="33">
-        <v>506</v>
-      </c>
-      <c r="D49" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="F49" s="32" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="35" t="s">
-        <v>108</v>
       </c>
       <c r="B50" s="35" t="s">
         <v>67</v>
       </c>
       <c r="C50" s="33">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D50" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E50" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="F50" s="32"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B51" s="35" t="s">
         <v>67</v>
       </c>
       <c r="C51" s="33">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D51" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E51" s="35" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F51" s="32"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B52" s="35" t="s">
         <v>67</v>
       </c>
       <c r="C52" s="33">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D52" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E52" s="35" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="F52" s="32"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B53" s="35" t="s">
         <v>67</v>
       </c>
       <c r="C53" s="33">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D53" s="34" t="s">
         <v>0</v>
@@ -2384,69 +2387,69 @@
       </c>
       <c r="F53" s="32"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="35" t="s">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="B54" s="35" t="s">
         <v>67</v>
       </c>
       <c r="C54" s="33">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D54" s="34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" s="35" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="F54" s="32"/>
     </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="35" t="s">
-        <v>197</v>
+        <v>40</v>
       </c>
       <c r="B55" s="35" t="s">
         <v>67</v>
       </c>
       <c r="C55" s="33">
+        <v>511</v>
+      </c>
+      <c r="D55" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E55" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F55" s="32"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="B56" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C56" s="33">
         <v>512</v>
       </c>
-      <c r="D55" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E55" s="35" t="s">
+      <c r="D56" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="F55" s="32"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="39" t="s">
+      <c r="F56" s="32"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="39" t="s">
         <v>112</v>
-      </c>
-      <c r="B56" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="C56" s="37">
-        <v>601</v>
-      </c>
-      <c r="D56" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="E56" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="36"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="39" t="s">
-        <v>113</v>
       </c>
       <c r="B57" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C57" s="37">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D57" s="38" t="s">
         <v>0</v>
@@ -2456,217 +2459,217 @@
       </c>
       <c r="F57" s="36"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B58" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C58" s="37">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D58" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E58" s="39" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="F58" s="36"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="39" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B59" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C59" s="37">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D59" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59" s="39" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
       <c r="F59" s="36"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B60" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C60" s="37">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D60" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60" s="39" t="s">
         <v>116</v>
       </c>
       <c r="F60" s="36"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="39" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="B61" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C61" s="37">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D61" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="F61" s="36" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="F61" s="36"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="39" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B62" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C62" s="37">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D62" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E62" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="F62" s="36"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="F62" s="36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="39" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="B63" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C63" s="37">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D63" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E63" s="39" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F63" s="36"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="39" t="s">
-        <v>120</v>
+        <v>43</v>
       </c>
       <c r="B64" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C64" s="37">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D64" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E64" s="39" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F64" s="36"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B65" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C65" s="37">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D65" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" s="39" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="F65" s="36"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B66" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C66" s="37">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D66" s="38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66" s="39" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F66" s="36"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="39" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B67" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C67" s="37">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D67" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E67" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="F67" s="36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="F67" s="36"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="39" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="B68" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C68" s="37">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D68" s="38" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="F68" s="36"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F68" s="36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B69" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C69" s="37">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D69" s="38" t="s">
         <v>0</v>
@@ -2676,33 +2679,33 @@
       </c>
       <c r="F69" s="36"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B70" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C70" s="37">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D70" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E70" s="39" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F70" s="36"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B71" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C71" s="37">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D71" s="38" t="s">
         <v>0</v>
@@ -2712,255 +2715,253 @@
       </c>
       <c r="F71" s="36"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="39" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B72" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C72" s="37">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D72" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E72" s="39" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F72" s="36"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="39" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B73" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C73" s="37">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D73" s="38" t="s">
         <v>0</v>
       </c>
       <c r="E73" s="39" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="F73" s="36"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="53" t="s">
-        <v>194</v>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="39" t="s">
+        <v>173</v>
       </c>
       <c r="B74" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C74" s="37">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D74" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E74" s="51" t="s">
-        <v>27</v>
+      <c r="E74" s="39" t="s">
+        <v>174</v>
       </c>
       <c r="F74" s="36"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="53" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B75" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C75" s="37">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D75" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E75" s="54" t="s">
-        <v>201</v>
+      <c r="E75" s="51" t="s">
+        <v>27</v>
       </c>
       <c r="F75" s="36"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="55" t="s">
-        <v>202</v>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="53" t="s">
+        <v>200</v>
       </c>
       <c r="B76" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C76" s="37">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D76" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E76" s="53" t="s">
-        <v>51</v>
+      <c r="E76" s="54" t="s">
+        <v>201</v>
       </c>
       <c r="F76" s="36"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="55" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B77" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C77" s="37">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D77" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E77" s="56" t="s">
-        <v>205</v>
+      <c r="E77" s="53" t="s">
+        <v>51</v>
       </c>
       <c r="F77" s="36"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="55" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B78" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C78" s="37">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D78" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E78" s="57" t="s">
-        <v>161</v>
+      <c r="E78" s="56" t="s">
+        <v>205</v>
       </c>
       <c r="F78" s="36"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="55" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B79" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C79" s="37">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D79" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="E79" s="55" t="s">
-        <v>163</v>
+      <c r="E79" s="57" t="s">
+        <v>161</v>
       </c>
       <c r="F79" s="36"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="58" t="s">
-        <v>215</v>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="55" t="s">
+        <v>209</v>
       </c>
       <c r="B80" s="39" t="s">
         <v>70</v>
       </c>
       <c r="C80" s="37">
+        <v>624</v>
+      </c>
+      <c r="D80" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E80" s="55" t="s">
+        <v>163</v>
+      </c>
+      <c r="F80" s="36"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="B81" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C81" s="37">
         <v>625</v>
       </c>
-      <c r="D80" s="38" t="s">
+      <c r="D81" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="E80" s="59" t="s">
+      <c r="E81" s="59" t="s">
         <v>199</v>
       </c>
-      <c r="F80" s="36" t="s">
+      <c r="F81" s="36" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="27" t="s">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="27" t="s">
         <v>124</v>
-      </c>
-      <c r="B81" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C81" s="25">
-        <v>701</v>
-      </c>
-      <c r="D81" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E81" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F81" s="24"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="27" t="s">
-        <v>115</v>
       </c>
       <c r="B82" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C82" s="25">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D82" s="26" t="s">
         <v>61</v>
       </c>
       <c r="E82" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F82" s="24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F82" s="24"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="27" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B83" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C83" s="25">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D83" s="26" t="s">
         <v>61</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F83" s="24"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B84" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C84" s="25">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E84" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F84" s="24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="F84" s="24"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B85" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C85" s="25">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D85" s="26" t="s">
         <v>0</v>
@@ -2972,15 +2973,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B86" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C86" s="25">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D86" s="26" t="s">
         <v>0</v>
@@ -2989,18 +2990,18 @@
         <v>10</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B87" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C87" s="25">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D87" s="26" t="s">
         <v>0</v>
@@ -3012,15 +3013,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B88" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C88" s="25">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D88" s="26" t="s">
         <v>0</v>
@@ -3029,18 +3030,18 @@
         <v>10</v>
       </c>
       <c r="F88" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B89" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C89" s="25">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D89" s="26" t="s">
         <v>0</v>
@@ -3052,573 +3053,593 @@
         <v>13</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B90" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C90" s="25">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D90" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E90" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F90" s="24"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="F90" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B91" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C91" s="25">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D91" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E91" s="27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F91" s="24"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="27" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="B92" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C92" s="25">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D92" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E92" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F92" s="24"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="27" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="B93" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C93" s="25">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D93" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E93" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F93" s="24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="F93" s="24"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B94" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C94" s="25">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D94" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E94" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="F94" s="24"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="F94" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B95" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C95" s="25">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D95" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E95" s="27" t="s">
-        <v>50</v>
+        <v>164</v>
       </c>
       <c r="F95" s="24"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B96" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C96" s="25">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D96" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F96" s="24"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="27" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B97" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C97" s="25">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D97" s="26" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="E97" s="27" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F97" s="24"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="27" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="B98" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C98" s="25">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D98" s="26" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E98" s="27" t="s">
-        <v>175</v>
+        <v>29</v>
       </c>
       <c r="F98" s="24"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="27" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B99" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C99" s="25">
+        <v>718</v>
+      </c>
+      <c r="D99" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E99" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="F99" s="24"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B100" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C100" s="25">
         <v>719</v>
       </c>
-      <c r="D99" s="26" t="s">
+      <c r="D100" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E99" s="27" t="s">
+      <c r="E100" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="F99" s="24"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="43" t="s">
+      <c r="F100" s="24"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="43" t="s">
         <v>198</v>
-      </c>
-      <c r="B100" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C100" s="41">
-        <v>801</v>
-      </c>
-      <c r="D100" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E100" s="43" t="s">
-        <v>199</v>
-      </c>
-      <c r="F100" s="40"/>
-    </row>
-    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="43" t="s">
-        <v>42</v>
       </c>
       <c r="B101" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C101" s="41">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D101" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E101" s="43" t="s">
-        <v>54</v>
+        <v>199</v>
       </c>
       <c r="F101" s="40"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A102" s="43" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B102" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C102" s="41">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D102" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E102" s="43" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F102" s="40"/>
     </row>
-    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B103" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C103" s="41">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D103" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E103" s="43" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F103" s="40"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A104" s="43" t="s">
-        <v>138</v>
+        <v>47</v>
       </c>
       <c r="B104" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C104" s="41">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D104" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E104" s="43" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F104" s="40"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="43" t="s">
-        <v>204</v>
+        <v>138</v>
       </c>
       <c r="B105" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C105" s="41">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D105" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E105" s="43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F105" s="40"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="43" t="s">
-        <v>52</v>
+        <v>204</v>
       </c>
       <c r="B106" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C106" s="41">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D106" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E106" s="43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F106" s="40"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="43" t="s">
-        <v>139</v>
+        <v>52</v>
       </c>
       <c r="B107" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C107" s="41">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D107" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E107" s="43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F107" s="40"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="43" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="B108" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C108" s="41">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D108" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E108" s="43" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F108" s="40"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B109" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C109" s="41">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D109" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E109" s="43" t="s">
-        <v>157</v>
+        <v>48</v>
       </c>
       <c r="F109" s="40"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B110" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C110" s="41">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D110" s="42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110" s="43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F110" s="40"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B111" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C111" s="41">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D111" s="42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111" s="43" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F111" s="40"/>
     </row>
-    <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="43" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B112" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C112" s="41">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D112" s="42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112" s="43" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F112" s="40"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A113" s="43" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="B113" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C113" s="41">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D113" s="42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113" s="43" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="F113" s="40"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="43" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B114" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C114" s="41">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D114" s="42" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="E114" s="43" t="s">
-        <v>190</v>
+        <v>18</v>
       </c>
       <c r="F114" s="40"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="43" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="B115" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C115" s="41">
+        <v>815</v>
+      </c>
+      <c r="D115" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E115" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="F115" s="40"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="B116" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C116" s="41">
         <v>816</v>
       </c>
-      <c r="D115" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E115" s="43" t="s">
+      <c r="D116" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E116" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="F115" s="40"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="47" t="s">
+      <c r="F116" s="40"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="47" t="s">
         <v>28</v>
-      </c>
-      <c r="B116" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="C116" s="45">
-        <v>901</v>
-      </c>
-      <c r="D116" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="E116" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="F116" s="44"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="47" t="s">
-        <v>144</v>
       </c>
       <c r="B117" s="47" t="s">
         <v>68</v>
       </c>
       <c r="C117" s="45">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D117" s="46" t="s">
         <v>61</v>
       </c>
       <c r="E117" s="47" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F117" s="44"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="47" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B118" s="47" t="s">
         <v>68</v>
       </c>
       <c r="C118" s="45">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D118" s="46" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E118" s="47" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="F118" s="44"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B119" s="47" t="s">
         <v>68</v>
       </c>
       <c r="C119" s="45">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D119" s="46" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="E119" s="47" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F119" s="44"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="47" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B120" s="47" t="s">
         <v>68</v>
       </c>
       <c r="C120" s="45">
+        <v>904</v>
+      </c>
+      <c r="D120" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="E120" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="F120" s="44"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B121" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C121" s="45">
         <v>905</v>
       </c>
-      <c r="D120" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E120" s="47" t="s">
+      <c r="D121" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E121" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="F120" s="44"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="1"/>
-      <c r="E121" s="2"/>
-      <c r="F121" s="1"/>
+      <c r="F121" s="44"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="2"/>
+      <c r="B122" s="2"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:E69">

</xml_diff>

<commit_message>
Introduce constant objects for literals in pattern expressions fixed idioms
</commit_message>
<xml_diff>
--- a/elevator_log_messages.xlsx
+++ b/elevator_log_messages.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22820" windowHeight="17160" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22820" windowHeight="16660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Error Codes - STIX Elevator" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="221">
   <si>
     <t>warn</t>
   </si>
@@ -684,6 +684,12 @@
   </si>
   <si>
     <t>silent option is not compatible with a policy</t>
+  </si>
+  <si>
+    <t>convert_hashes_to_pattern</t>
+  </si>
+  <si>
+    <t>"'[hash_string]' is not a valid [hash_type] hash"</t>
   </si>
 </sst>
 </file>
@@ -732,6 +738,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -752,6 +759,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -759,6 +767,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -884,7 +893,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="60">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -917,6 +926,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1072,7 +1083,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="31" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="31" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="60">
+  <cellStyles count="62">
     <cellStyle name="20% - Accent2" xfId="31" builtinId="34"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1103,6 +1114,7 @@
     <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1132,6 +1144,7 @@
     <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1415,10 +1428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F122"/>
+  <dimension ref="A1:F123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2898,90 +2911,88 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="B82" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C82" s="25">
-        <v>701</v>
-      </c>
-      <c r="D82" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="E82" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="F82" s="24"/>
+      <c r="A82" s="58" t="s">
+        <v>220</v>
+      </c>
+      <c r="B82" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C82" s="37">
+        <v>626</v>
+      </c>
+      <c r="D82" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="F82" s="36"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="27" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B83" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C83" s="25">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="D83" s="26" t="s">
         <v>61</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F83" s="24" t="s">
-        <v>39</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F83" s="24"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="27" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B84" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C84" s="25">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D84" s="26" t="s">
         <v>61</v>
       </c>
       <c r="E84" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F84" s="24"/>
+        <v>38</v>
+      </c>
+      <c r="F84" s="24" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B85" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C85" s="25">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F85" s="24" t="s">
-        <v>11</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="F85" s="24"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="27" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B86" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C86" s="25">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D86" s="26" t="s">
         <v>0</v>
@@ -2995,13 +3006,13 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B87" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C87" s="25">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D87" s="26" t="s">
         <v>0</v>
@@ -3010,18 +3021,18 @@
         <v>10</v>
       </c>
       <c r="F87" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B88" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C88" s="25">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D88" s="26" t="s">
         <v>0</v>
@@ -3035,13 +3046,13 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B89" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C89" s="25">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D89" s="26" t="s">
         <v>0</v>
@@ -3050,18 +3061,18 @@
         <v>10</v>
       </c>
       <c r="F89" s="24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B90" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C90" s="25">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D90" s="26" t="s">
         <v>0</v>
@@ -3075,571 +3086,591 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="27" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B91" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C91" s="25">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D91" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E91" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F91" s="24"/>
+        <v>10</v>
+      </c>
+      <c r="F91" s="24" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B92" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C92" s="25">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D92" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E92" s="27" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F92" s="24"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="27" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="B93" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C93" s="25">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D93" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E93" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F93" s="24"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="27" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="B94" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C94" s="25">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D94" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E94" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F94" s="24" t="s">
-        <v>35</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F94" s="24"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B95" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C95" s="25">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D95" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E95" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="F95" s="24"/>
+        <v>34</v>
+      </c>
+      <c r="F95" s="24" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B96" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C96" s="25">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D96" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>50</v>
+        <v>164</v>
       </c>
       <c r="F96" s="24"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B97" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C97" s="25">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D97" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E97" s="27" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F97" s="24"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="27" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B98" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C98" s="25">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D98" s="26" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="E98" s="27" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F98" s="24"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="27" t="s">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="B99" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C99" s="25">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D99" s="26" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E99" s="27" t="s">
-        <v>175</v>
+        <v>29</v>
       </c>
       <c r="F99" s="24"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="27" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B100" s="27" t="s">
         <v>69</v>
       </c>
       <c r="C100" s="25">
+        <v>718</v>
+      </c>
+      <c r="D100" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E100" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="F100" s="24"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B101" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C101" s="25">
         <v>719</v>
       </c>
-      <c r="D100" s="26" t="s">
+      <c r="D101" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E100" s="27" t="s">
+      <c r="E101" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="F100" s="24"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="43" t="s">
+      <c r="F101" s="24"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="43" t="s">
         <v>198</v>
-      </c>
-      <c r="B101" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C101" s="41">
-        <v>801</v>
-      </c>
-      <c r="D101" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E101" s="43" t="s">
-        <v>199</v>
-      </c>
-      <c r="F101" s="40"/>
-    </row>
-    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A102" s="43" t="s">
-        <v>42</v>
       </c>
       <c r="B102" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C102" s="41">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D102" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E102" s="43" t="s">
-        <v>54</v>
+        <v>199</v>
       </c>
       <c r="F102" s="40"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A103" s="43" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B103" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C103" s="41">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D103" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E103" s="43" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F103" s="40"/>
     </row>
-    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B104" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C104" s="41">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D104" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E104" s="43" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F104" s="40"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A105" s="43" t="s">
-        <v>138</v>
+        <v>47</v>
       </c>
       <c r="B105" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C105" s="41">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D105" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E105" s="43" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="F105" s="40"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="43" t="s">
-        <v>204</v>
+        <v>138</v>
       </c>
       <c r="B106" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C106" s="41">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D106" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E106" s="43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F106" s="40"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="43" t="s">
-        <v>52</v>
+        <v>204</v>
       </c>
       <c r="B107" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C107" s="41">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D107" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E107" s="43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F107" s="40"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="43" t="s">
-        <v>139</v>
+        <v>52</v>
       </c>
       <c r="B108" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C108" s="41">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D108" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E108" s="43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F108" s="40"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="43" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="B109" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C109" s="41">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D109" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E109" s="43" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F109" s="40"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B110" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C110" s="41">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D110" s="42" t="s">
         <v>0</v>
       </c>
       <c r="E110" s="43" t="s">
-        <v>157</v>
+        <v>48</v>
       </c>
       <c r="F110" s="40"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B111" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C111" s="41">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D111" s="42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E111" s="43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F111" s="40"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B112" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C112" s="41">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D112" s="42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112" s="43" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F112" s="40"/>
     </row>
-    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="43" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B113" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C113" s="41">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D113" s="42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E113" s="43" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F113" s="40"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A114" s="43" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="B114" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C114" s="41">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D114" s="42" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E114" s="43" t="s">
-        <v>18</v>
+        <v>166</v>
       </c>
       <c r="F114" s="40"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="43" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B115" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C115" s="41">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D115" s="42" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="E115" s="43" t="s">
-        <v>190</v>
+        <v>18</v>
       </c>
       <c r="F115" s="40"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="43" t="s">
-        <v>214</v>
+        <v>189</v>
       </c>
       <c r="B116" s="43" t="s">
         <v>63</v>
       </c>
       <c r="C116" s="41">
+        <v>815</v>
+      </c>
+      <c r="D116" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E116" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="F116" s="40"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="B117" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C117" s="41">
         <v>816</v>
       </c>
-      <c r="D116" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E116" s="43" t="s">
+      <c r="D117" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E117" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="F116" s="40"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B117" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="C117" s="45">
-        <v>901</v>
-      </c>
-      <c r="D117" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="E117" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="F117" s="44"/>
+      <c r="F117" s="40"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="47" t="s">
-        <v>144</v>
+        <v>28</v>
       </c>
       <c r="B118" s="47" t="s">
         <v>68</v>
       </c>
       <c r="C118" s="45">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D118" s="46" t="s">
         <v>61</v>
       </c>
       <c r="E118" s="47" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F118" s="44"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="47" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B119" s="47" t="s">
         <v>68</v>
       </c>
       <c r="C119" s="45">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D119" s="46" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="E119" s="47" t="s">
-        <v>27</v>
+        <v>145</v>
       </c>
       <c r="F119" s="44"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B120" s="47" t="s">
         <v>68</v>
       </c>
       <c r="C120" s="45">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D120" s="46" t="s">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="E120" s="47" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F120" s="44"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="47" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B121" s="47" t="s">
         <v>68</v>
       </c>
       <c r="C121" s="45">
+        <v>904</v>
+      </c>
+      <c r="D121" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="E121" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="F121" s="44"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="B122" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="C122" s="45">
         <v>905</v>
       </c>
-      <c r="D121" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="E121" s="47" t="s">
+      <c r="D122" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="E122" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="F121" s="44"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122" s="2"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="1"/>
-      <c r="E122" s="2"/>
-      <c r="F122" s="1"/>
+      <c r="F122" s="44"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="2"/>
+      <c r="B123" s="2"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="1"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="1"/>
     </row>
   </sheetData>
   <sortState ref="A1:E69">

</xml_diff>